<commit_message>
Updated on 04-30-2024 at 20:43
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,13 +458,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3484</v>
+        <v>0.02677</v>
       </c>
       <c r="D2" t="n">
-        <v>3.461</v>
+        <v>1.144</v>
       </c>
       <c r="E2" t="n">
-        <v>1.715</v>
+        <v>2.38</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
@@ -478,13 +478,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3856</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>4.056</v>
+        <v>1.416</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6059</v>
+        <v>1.819</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>
@@ -498,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4139</v>
+        <v>0.0346</v>
       </c>
       <c r="D4" t="n">
-        <v>4.408</v>
+        <v>1.884</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8223</v>
+        <v>1.742</v>
       </c>
       <c r="F4" t="n">
         <v>5</v>
@@ -518,13 +518,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3308</v>
+        <v>0.0005845</v>
       </c>
       <c r="D5" t="n">
-        <v>4.616</v>
+        <v>2.189</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1534</v>
+        <v>1.121</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
@@ -538,13 +538,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1351</v>
+        <v>0.008944000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>4.814</v>
+        <v>2.462</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1706</v>
+        <v>0.4541</v>
       </c>
       <c r="F6" t="n">
         <v>5</v>
@@ -558,16 +558,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1351</v>
+        <v>0.002097</v>
       </c>
       <c r="D7" t="n">
-        <v>1.168</v>
+        <v>2.708</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4955</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -578,13 +578,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2847</v>
+        <v>4.872e-05</v>
       </c>
       <c r="D8" t="n">
-        <v>3.683</v>
+        <v>2.032</v>
       </c>
       <c r="E8" t="n">
-        <v>2.671</v>
+        <v>1.225</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
@@ -598,13 +598,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2426</v>
+        <v>0.006281</v>
       </c>
       <c r="D9" t="n">
-        <v>4.398</v>
+        <v>2.769</v>
       </c>
       <c r="E9" t="n">
-        <v>2.182</v>
+        <v>1.321</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>
@@ -618,13 +618,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4646</v>
+        <v>0.04933</v>
       </c>
       <c r="D10" t="n">
-        <v>4.819</v>
+        <v>3.006</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5923</v>
+        <v>0.9503</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -638,16 +638,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4228</v>
+        <v>0.04533</v>
       </c>
       <c r="D11" t="n">
-        <v>20.35</v>
+        <v>2.871</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1071</v>
+        <v>0.8944</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -658,13 +658,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3204</v>
+        <v>0.001937</v>
       </c>
       <c r="D12" t="n">
-        <v>8.180999999999999</v>
+        <v>2.91</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7953</v>
+        <v>0.6382</v>
       </c>
       <c r="F12" t="n">
         <v>5</v>
@@ -678,13 +678,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2761</v>
+        <v>0.001944</v>
       </c>
       <c r="D13" t="n">
-        <v>5.828</v>
+        <v>2.898</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9553</v>
+        <v>0.5722</v>
       </c>
       <c r="F13" t="n">
         <v>5</v>
@@ -698,16 +698,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2507</v>
+        <v>0.2761</v>
       </c>
       <c r="D14" t="n">
-        <v>5.59</v>
+        <v>2.331</v>
       </c>
       <c r="E14" t="n">
-        <v>1.361</v>
+        <v>0.2538</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
@@ -718,16 +718,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.09676999999999999</v>
+        <v>0.1313</v>
       </c>
       <c r="D15" t="n">
-        <v>5.842</v>
+        <v>2.487</v>
       </c>
       <c r="E15" t="n">
-        <v>1.121</v>
+        <v>0.2041</v>
       </c>
       <c r="F15" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -738,13 +738,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0486</v>
+        <v>0.0005012</v>
       </c>
       <c r="D16" t="n">
-        <v>6.178</v>
+        <v>3.475</v>
       </c>
       <c r="E16" t="n">
-        <v>1.278</v>
+        <v>0.4351</v>
       </c>
       <c r="F16" t="n">
         <v>5</v>
@@ -758,13 +758,13 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.03915</v>
+        <v>4.638e-07</v>
       </c>
       <c r="D17" t="n">
-        <v>6.546</v>
+        <v>3.888</v>
       </c>
       <c r="E17" t="n">
-        <v>1.675</v>
+        <v>0.844</v>
       </c>
       <c r="F17" t="n">
         <v>5</v>
@@ -778,13 +778,13 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1849</v>
+        <v>8.296000000000001e-05</v>
       </c>
       <c r="D18" t="n">
-        <v>6.738</v>
+        <v>4.028</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9827</v>
+        <v>0.9012</v>
       </c>
       <c r="F18" t="n">
         <v>5</v>
@@ -798,16 +798,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0003701</v>
+        <v>0.02765</v>
       </c>
       <c r="D19" t="n">
-        <v>7.075</v>
+        <v>2.943</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2202</v>
+        <v>0.5685</v>
       </c>
       <c r="F19" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -818,13 +818,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1365</v>
+        <v>0.0007654</v>
       </c>
       <c r="D20" t="n">
-        <v>7.341</v>
+        <v>4.617</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2463</v>
+        <v>1.179</v>
       </c>
       <c r="F20" t="n">
         <v>5</v>
@@ -838,13 +838,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.07922999999999999</v>
+        <v>0.0006609</v>
       </c>
       <c r="D21" t="n">
-        <v>7.604</v>
+        <v>4.968</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3729</v>
+        <v>1.323</v>
       </c>
       <c r="F21" t="n">
         <v>5</v>
@@ -858,13 +858,13 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.029</v>
+        <v>0.007643</v>
       </c>
       <c r="D22" t="n">
-        <v>7.768</v>
+        <v>5.16</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3875</v>
+        <v>1.304</v>
       </c>
       <c r="F22" t="n">
         <v>5</v>
@@ -878,13 +878,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.03624</v>
+        <v>0.003798</v>
       </c>
       <c r="D23" t="n">
-        <v>7.77</v>
+        <v>5.25</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4257</v>
+        <v>0.7727000000000001</v>
       </c>
       <c r="F23" t="n">
         <v>5</v>
@@ -898,13 +898,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01635</v>
+        <v>0.0002045</v>
       </c>
       <c r="D24" t="n">
-        <v>7.847</v>
+        <v>5.529</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6127</v>
+        <v>0.5427</v>
       </c>
       <c r="F24" t="n">
         <v>5</v>
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01474</v>
+        <v>0.03006</v>
       </c>
       <c r="D25" t="n">
-        <v>7.854</v>
+        <v>4.23</v>
       </c>
       <c r="E25" t="n">
-        <v>0.841</v>
+        <v>0.05253</v>
       </c>
       <c r="F25" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26">
@@ -938,16 +938,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.02436</v>
+        <v>0.03846</v>
       </c>
       <c r="D26" t="n">
-        <v>22.99</v>
+        <v>4.002</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3336</v>
+        <v>0.146</v>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
@@ -958,13 +958,13 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.03638</v>
+        <v>0.0008876999999999999</v>
       </c>
       <c r="D27" t="n">
-        <v>10.82</v>
+        <v>5.346</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5809</v>
+        <v>0.4769</v>
       </c>
       <c r="F27" t="n">
         <v>5</v>
@@ -978,13 +978,13 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01533</v>
+        <v>0.00139</v>
       </c>
       <c r="D28" t="n">
-        <v>8.285</v>
+        <v>5.644</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7125</v>
+        <v>0.8708</v>
       </c>
       <c r="F28" t="n">
         <v>5</v>
@@ -998,13 +998,13 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0197</v>
+        <v>0.001937</v>
       </c>
       <c r="D29" t="n">
-        <v>7.766</v>
+        <v>5.772</v>
       </c>
       <c r="E29" t="n">
-        <v>0.4791</v>
+        <v>0.9781</v>
       </c>
       <c r="F29" t="n">
         <v>5</v>
@@ -1018,13 +1018,13 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.02576</v>
+        <v>0.0002671</v>
       </c>
       <c r="D30" t="n">
-        <v>7.659</v>
+        <v>5.768</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3386</v>
+        <v>1.092</v>
       </c>
       <c r="F30" t="n">
         <v>5</v>
@@ -1038,16 +1038,16 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.06807000000000001</v>
+        <v>0.0001061</v>
       </c>
       <c r="D31" t="n">
-        <v>22.85</v>
+        <v>5.86</v>
       </c>
       <c r="E31" t="n">
-        <v>0.253</v>
+        <v>0.8046</v>
       </c>
       <c r="F31" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -1058,13 +1058,13 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.03512</v>
+        <v>0.0002671</v>
       </c>
       <c r="D32" t="n">
-        <v>10.92</v>
+        <v>5.846</v>
       </c>
       <c r="E32" t="n">
-        <v>0.922</v>
+        <v>0.2972</v>
       </c>
       <c r="F32" t="n">
         <v>5</v>
@@ -1078,13 +1078,13 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.02777</v>
+        <v>0.0004712</v>
       </c>
       <c r="D33" t="n">
-        <v>8.528</v>
+        <v>5.749</v>
       </c>
       <c r="E33" t="n">
-        <v>0.7369</v>
+        <v>0.4281</v>
       </c>
       <c r="F33" t="n">
         <v>5</v>
@@ -1098,16 +1098,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01168</v>
+        <v>0.02777</v>
       </c>
       <c r="D34" t="n">
-        <v>8.275</v>
+        <v>5.092</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9738</v>
+        <v>0.0883</v>
       </c>
       <c r="F34" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35">
@@ -1118,13 +1118,13 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0094</v>
+        <v>0.001494</v>
       </c>
       <c r="D35" t="n">
-        <v>8.387</v>
+        <v>5.901</v>
       </c>
       <c r="E35" t="n">
-        <v>1.074</v>
+        <v>0.4095</v>
       </c>
       <c r="F35" t="n">
         <v>5</v>
@@ -1138,13 +1138,13 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0.02471</v>
+        <v>0.002922</v>
       </c>
       <c r="D36" t="n">
-        <v>8.513</v>
+        <v>6.127</v>
       </c>
       <c r="E36" t="n">
-        <v>1.065</v>
+        <v>0.8233</v>
       </c>
       <c r="F36" t="n">
         <v>5</v>
@@ -1158,13 +1158,13 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.07881000000000001</v>
+        <v>0.0006306</v>
       </c>
       <c r="D37" t="n">
-        <v>8.435</v>
+        <v>6.089</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2847</v>
+        <v>0.6877</v>
       </c>
       <c r="F37" t="n">
         <v>5</v>
@@ -1178,13 +1178,13 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.06856</v>
+        <v>0.0001719</v>
       </c>
       <c r="D38" t="n">
-        <v>8.345000000000001</v>
+        <v>6.185</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4637</v>
+        <v>0.476</v>
       </c>
       <c r="F38" t="n">
         <v>5</v>
@@ -1198,13 +1198,13 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.03904</v>
+        <v>0.001069</v>
       </c>
       <c r="D39" t="n">
-        <v>8.318</v>
+        <v>6.335</v>
       </c>
       <c r="E39" t="n">
-        <v>0.7395</v>
+        <v>0.4138</v>
       </c>
       <c r="F39" t="n">
         <v>5</v>
@@ -1218,13 +1218,13 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.02613</v>
+        <v>0.0002812</v>
       </c>
       <c r="D40" t="n">
-        <v>8.265000000000001</v>
+        <v>6.341</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8516</v>
+        <v>0.3649</v>
       </c>
       <c r="F40" t="n">
         <v>5</v>
@@ -1238,16 +1238,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.01964</v>
+        <v>0.02613</v>
       </c>
       <c r="D41" t="n">
-        <v>8.099</v>
+        <v>5.043</v>
       </c>
       <c r="E41" t="n">
-        <v>1.042</v>
+        <v>0.037</v>
       </c>
       <c r="F41" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42">
@@ -1258,13 +1258,13 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01761</v>
+        <v>7.890999999999999e-06</v>
       </c>
       <c r="D42" t="n">
-        <v>7.994</v>
+        <v>5.954</v>
       </c>
       <c r="E42" t="n">
-        <v>1.246</v>
+        <v>0.6072</v>
       </c>
       <c r="F42" t="n">
         <v>5</v>
@@ -1278,16 +1278,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.006423</v>
+        <v>0.4577</v>
       </c>
       <c r="D43" t="n">
-        <v>4.505</v>
+        <v>5.047</v>
       </c>
       <c r="E43" t="n">
-        <v>0.2819</v>
+        <v>0.4592</v>
       </c>
       <c r="F43" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44">
@@ -1298,13 +1298,13 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.229</v>
+        <v>0.0002045</v>
       </c>
       <c r="D44" t="n">
-        <v>8.257</v>
+        <v>6.582</v>
       </c>
       <c r="E44" t="n">
-        <v>1.989</v>
+        <v>0.5487</v>
       </c>
       <c r="F44" t="n">
         <v>5</v>
@@ -1318,13 +1318,13 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1419</v>
+        <v>0.002354</v>
       </c>
       <c r="D45" t="n">
-        <v>9.221</v>
+        <v>6.634</v>
       </c>
       <c r="E45" t="n">
-        <v>2.506</v>
+        <v>0.9028</v>
       </c>
       <c r="F45" t="n">
         <v>5</v>
@@ -1338,13 +1338,13 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1138</v>
+        <v>0.00129</v>
       </c>
       <c r="D46" t="n">
-        <v>9.414999999999999</v>
+        <v>6.625</v>
       </c>
       <c r="E46" t="n">
-        <v>2.1</v>
+        <v>0.8683999999999999</v>
       </c>
       <c r="F46" t="n">
         <v>5</v>
@@ -1358,13 +1358,13 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1082</v>
+        <v>0.00479</v>
       </c>
       <c r="D47" t="n">
-        <v>9.353999999999999</v>
+        <v>6.751</v>
       </c>
       <c r="E47" t="n">
-        <v>0.8519</v>
+        <v>0.483</v>
       </c>
       <c r="F47" t="n">
         <v>5</v>
@@ -1378,16 +1378,16 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1082</v>
+        <v>3.551e-05</v>
       </c>
       <c r="D48" t="n">
-        <v>4.916</v>
+        <v>7.113</v>
       </c>
       <c r="E48" t="n">
-        <v>0.144</v>
+        <v>0.5113</v>
       </c>
       <c r="F48" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.3227</v>
+        <v>8.609e-05</v>
       </c>
       <c r="D49" t="n">
-        <v>23.7</v>
+        <v>7.171</v>
       </c>
       <c r="E49" t="n">
-        <v>0.7191</v>
+        <v>0.6042</v>
       </c>
       <c r="F49" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -1418,16 +1418,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.2471</v>
+        <v>0.1182</v>
       </c>
       <c r="D50" t="n">
-        <v>11.54</v>
+        <v>5.289</v>
       </c>
       <c r="E50" t="n">
-        <v>2.329</v>
+        <v>0.3804</v>
       </c>
       <c r="F50" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51">
@@ -1438,13 +1438,13 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>0.1853</v>
+        <v>1.403e-05</v>
       </c>
       <c r="D51" t="n">
-        <v>8.605</v>
+        <v>6.289</v>
       </c>
       <c r="E51" t="n">
-        <v>3.537</v>
+        <v>1.102</v>
       </c>
       <c r="F51" t="n">
         <v>5</v>
@@ -1458,13 +1458,13 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>0.1655</v>
+        <v>0.003351</v>
       </c>
       <c r="D52" t="n">
-        <v>7.787</v>
+        <v>6.51</v>
       </c>
       <c r="E52" t="n">
-        <v>3.006</v>
+        <v>1.376</v>
       </c>
       <c r="F52" t="n">
         <v>5</v>
@@ -1478,13 +1478,13 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1402</v>
+        <v>0.0003045</v>
       </c>
       <c r="D53" t="n">
-        <v>7.453</v>
+        <v>6.332</v>
       </c>
       <c r="E53" t="n">
-        <v>2.212</v>
+        <v>1.739</v>
       </c>
       <c r="F53" t="n">
         <v>5</v>
@@ -1498,13 +1498,13 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.6843</v>
+        <v>0.001467</v>
       </c>
       <c r="D54" t="n">
-        <v>7.508</v>
+        <v>6.269</v>
       </c>
       <c r="E54" t="n">
-        <v>0.4235</v>
+        <v>1.21</v>
       </c>
       <c r="F54" t="n">
         <v>5</v>
@@ -1518,13 +1518,13 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.3566</v>
+        <v>0.001435</v>
       </c>
       <c r="D55" t="n">
-        <v>7.459</v>
+        <v>5.811</v>
       </c>
       <c r="E55" t="n">
-        <v>1.096</v>
+        <v>0.9405</v>
       </c>
       <c r="F55" t="n">
         <v>5</v>
@@ -1538,13 +1538,13 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1492</v>
+        <v>0.003602</v>
       </c>
       <c r="D56" t="n">
-        <v>7.268</v>
+        <v>5.425</v>
       </c>
       <c r="E56" t="n">
-        <v>1.331</v>
+        <v>1.215</v>
       </c>
       <c r="F56" t="n">
         <v>5</v>
@@ -1558,13 +1558,13 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.1218</v>
+        <v>0.002066</v>
       </c>
       <c r="D57" t="n">
-        <v>7.357</v>
+        <v>5.557</v>
       </c>
       <c r="E57" t="n">
-        <v>1.968</v>
+        <v>0.4551</v>
       </c>
       <c r="F57" t="n">
         <v>5</v>
@@ -1578,13 +1578,13 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>0.1897</v>
+        <v>0.001003</v>
       </c>
       <c r="D58" t="n">
-        <v>7.19</v>
+        <v>5.238</v>
       </c>
       <c r="E58" t="n">
-        <v>1.268</v>
+        <v>0.4266</v>
       </c>
       <c r="F58" t="n">
         <v>5</v>
@@ -1598,13 +1598,13 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.243</v>
+        <v>0.008064999999999999</v>
       </c>
       <c r="D59" t="n">
-        <v>6.982</v>
+        <v>5.144</v>
       </c>
       <c r="E59" t="n">
-        <v>0.3571</v>
+        <v>0.5847</v>
       </c>
       <c r="F59" t="n">
         <v>5</v>
@@ -1618,13 +1618,13 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>0.2548</v>
+        <v>0.006485</v>
       </c>
       <c r="D60" t="n">
-        <v>7.009</v>
+        <v>5.281</v>
       </c>
       <c r="E60" t="n">
-        <v>0.2395</v>
+        <v>0.1414</v>
       </c>
       <c r="F60" t="n">
         <v>5</v>
@@ -1641,13 +1641,13 @@
         <v>0.2548</v>
       </c>
       <c r="D61" t="n">
-        <v>6.07</v>
+        <v>5.083</v>
       </c>
       <c r="E61" t="n">
-        <v>0.1818</v>
+        <v>0.191</v>
       </c>
       <c r="F61" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62">
@@ -1658,16 +1658,16 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>0.194</v>
+        <v>0.02748</v>
       </c>
       <c r="D62" t="n">
-        <v>6.801</v>
+        <v>4.555</v>
       </c>
       <c r="E62" t="n">
-        <v>0.1987</v>
+        <v>0.5453</v>
       </c>
       <c r="F62" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63">
@@ -1678,13 +1678,13 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1728</v>
+        <v>0.001621</v>
       </c>
       <c r="D63" t="n">
-        <v>7.642</v>
+        <v>5.397</v>
       </c>
       <c r="E63" t="n">
-        <v>0.9268999999999999</v>
+        <v>1.361</v>
       </c>
       <c r="F63" t="n">
         <v>5</v>
@@ -1698,13 +1698,13 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1054</v>
+        <v>0.0003016</v>
       </c>
       <c r="D64" t="n">
-        <v>7.995</v>
+        <v>5.459</v>
       </c>
       <c r="E64" t="n">
-        <v>1.142</v>
+        <v>1.516</v>
       </c>
       <c r="F64" t="n">
         <v>5</v>
@@ -1718,13 +1718,13 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.07396</v>
+        <v>0.001136</v>
       </c>
       <c r="D65" t="n">
-        <v>8.394</v>
+        <v>5.798</v>
       </c>
       <c r="E65" t="n">
-        <v>1.437</v>
+        <v>1.697</v>
       </c>
       <c r="F65" t="n">
         <v>5</v>
@@ -1738,13 +1738,13 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.06216</v>
+        <v>0.004142</v>
       </c>
       <c r="D66" t="n">
-        <v>8.943</v>
+        <v>6.247</v>
       </c>
       <c r="E66" t="n">
-        <v>2.165</v>
+        <v>2.258</v>
       </c>
       <c r="F66" t="n">
         <v>5</v>
@@ -1758,13 +1758,13 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>0.06906</v>
+        <v>0.0009496</v>
       </c>
       <c r="D67" t="n">
-        <v>9.242000000000001</v>
+        <v>6.376</v>
       </c>
       <c r="E67" t="n">
-        <v>1.611</v>
+        <v>2.06</v>
       </c>
       <c r="F67" t="n">
         <v>5</v>
@@ -1778,13 +1778,13 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1508</v>
+        <v>0.001266</v>
       </c>
       <c r="D68" t="n">
-        <v>9.397</v>
+        <v>6.621</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5243</v>
+        <v>1.491</v>
       </c>
       <c r="F68" t="n">
         <v>5</v>
@@ -1798,16 +1798,16 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1178</v>
+        <v>0.002644</v>
       </c>
       <c r="D69" t="n">
-        <v>24.5</v>
+        <v>6.99</v>
       </c>
       <c r="E69" t="n">
-        <v>0.2123</v>
+        <v>1.061</v>
       </c>
       <c r="F69" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1818,16 +1818,16 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.08351</v>
+        <v>4.899e-06</v>
       </c>
       <c r="D70" t="n">
-        <v>26.22</v>
+        <v>7.357</v>
       </c>
       <c r="E70" t="n">
-        <v>0.3495</v>
+        <v>0.9724</v>
       </c>
       <c r="F70" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71">
@@ -1838,16 +1838,36 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.03463</v>
+        <v>0.0002169</v>
       </c>
       <c r="D71" t="n">
-        <v>13.16</v>
+        <v>7.45</v>
       </c>
       <c r="E71" t="n">
-        <v>1.134</v>
+        <v>0.3644</v>
       </c>
       <c r="F71" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>71</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.6113</v>
+      </c>
+      <c r="D72" t="n">
+        <v>5.114</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.1405</v>
+      </c>
+      <c r="F72" t="n">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 04-30-2024 at 22:02
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -458,10 +458,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02677</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>1.144</v>
+        <v>1.246</v>
       </c>
       <c r="E2" t="n">
         <v>2.38</v>
@@ -478,10 +478,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.0346</v>
       </c>
       <c r="D3" t="n">
-        <v>1.416</v>
+        <v>1.711</v>
       </c>
       <c r="E3" t="n">
         <v>1.819</v>
@@ -498,10 +498,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0346</v>
+        <v>0.0005845</v>
       </c>
       <c r="D4" t="n">
-        <v>1.884</v>
+        <v>2.071</v>
       </c>
       <c r="E4" t="n">
         <v>1.742</v>
@@ -518,10 +518,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0005845</v>
+        <v>0.008944000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>2.189</v>
+        <v>2.283</v>
       </c>
       <c r="E5" t="n">
         <v>1.121</v>
@@ -538,10 +538,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.008944000000000001</v>
+        <v>0.002097</v>
       </c>
       <c r="D6" t="n">
-        <v>2.462</v>
+        <v>2.467</v>
       </c>
       <c r="E6" t="n">
         <v>0.4541</v>
@@ -558,10 +558,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.002097</v>
+        <v>4.872e-05</v>
       </c>
       <c r="D7" t="n">
-        <v>2.708</v>
+        <v>2.63</v>
       </c>
       <c r="E7" t="n">
         <v>0.9320000000000001</v>
@@ -578,10 +578,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>4.872e-05</v>
+        <v>0.006281</v>
       </c>
       <c r="D8" t="n">
-        <v>2.032</v>
+        <v>2.677</v>
       </c>
       <c r="E8" t="n">
         <v>1.225</v>
@@ -598,10 +598,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.006281</v>
+        <v>0.04933</v>
       </c>
       <c r="D9" t="n">
-        <v>2.769</v>
+        <v>2.71</v>
       </c>
       <c r="E9" t="n">
         <v>1.321</v>
@@ -618,10 +618,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.04933</v>
+        <v>0.04533</v>
       </c>
       <c r="D10" t="n">
-        <v>3.006</v>
+        <v>2.742</v>
       </c>
       <c r="E10" t="n">
         <v>0.9503</v>
@@ -638,10 +638,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.04533</v>
+        <v>0.001937</v>
       </c>
       <c r="D11" t="n">
-        <v>2.871</v>
+        <v>2.781</v>
       </c>
       <c r="E11" t="n">
         <v>0.8944</v>
@@ -658,10 +658,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.001937</v>
+        <v>0.001944</v>
       </c>
       <c r="D12" t="n">
-        <v>2.91</v>
+        <v>2.792</v>
       </c>
       <c r="E12" t="n">
         <v>0.6382</v>
@@ -678,10 +678,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.001944</v>
+        <v>0.0006522</v>
       </c>
       <c r="D13" t="n">
-        <v>2.898</v>
+        <v>2.94</v>
       </c>
       <c r="E13" t="n">
         <v>0.5722</v>
@@ -698,10 +698,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2761</v>
+        <v>0.2507</v>
       </c>
       <c r="D14" t="n">
-        <v>2.331</v>
+        <v>2.227</v>
       </c>
       <c r="E14" t="n">
         <v>0.2538</v>
@@ -718,10 +718,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1313</v>
+        <v>0.1076</v>
       </c>
       <c r="D15" t="n">
-        <v>2.487</v>
+        <v>2.284</v>
       </c>
       <c r="E15" t="n">
         <v>0.2041</v>
@@ -738,10 +738,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0005012</v>
+        <v>4.638e-07</v>
       </c>
       <c r="D16" t="n">
-        <v>3.475</v>
+        <v>3.349</v>
       </c>
       <c r="E16" t="n">
         <v>0.4351</v>
@@ -758,10 +758,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>4.638e-07</v>
+        <v>8.296000000000001e-05</v>
       </c>
       <c r="D17" t="n">
-        <v>3.888</v>
+        <v>3.802</v>
       </c>
       <c r="E17" t="n">
         <v>0.844</v>
@@ -778,10 +778,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>8.296000000000001e-05</v>
+        <v>0.0003701</v>
       </c>
       <c r="D18" t="n">
-        <v>4.028</v>
+        <v>4.139</v>
       </c>
       <c r="E18" t="n">
         <v>0.9012</v>
@@ -798,10 +798,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.02765</v>
+        <v>0.008718999999999999</v>
       </c>
       <c r="D19" t="n">
-        <v>2.943</v>
+        <v>3.081</v>
       </c>
       <c r="E19" t="n">
         <v>0.5685</v>
@@ -818,10 +818,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0007654</v>
+        <v>0.0006609</v>
       </c>
       <c r="D20" t="n">
-        <v>4.617</v>
+        <v>4.45</v>
       </c>
       <c r="E20" t="n">
         <v>1.179</v>
@@ -838,10 +838,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0006609</v>
+        <v>0.007643</v>
       </c>
       <c r="D21" t="n">
-        <v>4.968</v>
+        <v>4.945</v>
       </c>
       <c r="E21" t="n">
         <v>1.323</v>
@@ -858,10 +858,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.007643</v>
+        <v>0.003798</v>
       </c>
       <c r="D22" t="n">
-        <v>5.16</v>
+        <v>5.237</v>
       </c>
       <c r="E22" t="n">
         <v>1.304</v>
@@ -878,10 +878,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.003798</v>
+        <v>0.0002045</v>
       </c>
       <c r="D23" t="n">
-        <v>5.25</v>
+        <v>5.45</v>
       </c>
       <c r="E23" t="n">
         <v>0.7727000000000001</v>
@@ -898,10 +898,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0002045</v>
+        <v>0.0006052</v>
       </c>
       <c r="D24" t="n">
-        <v>5.529</v>
+        <v>5.654</v>
       </c>
       <c r="E24" t="n">
         <v>0.5427</v>
@@ -918,10 +918,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.03006</v>
+        <v>0.02814</v>
       </c>
       <c r="D25" t="n">
-        <v>4.23</v>
+        <v>4.409</v>
       </c>
       <c r="E25" t="n">
         <v>0.05253</v>
@@ -938,10 +938,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.03846</v>
+        <v>0.04602</v>
       </c>
       <c r="D26" t="n">
-        <v>4.002</v>
+        <v>4.106</v>
       </c>
       <c r="E26" t="n">
         <v>0.146</v>
@@ -958,10 +958,10 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0008876999999999999</v>
+        <v>0.00139</v>
       </c>
       <c r="D27" t="n">
-        <v>5.346</v>
+        <v>5.493</v>
       </c>
       <c r="E27" t="n">
         <v>0.4769</v>
@@ -978,10 +978,10 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.00139</v>
+        <v>0.001937</v>
       </c>
       <c r="D28" t="n">
-        <v>5.644</v>
+        <v>5.754</v>
       </c>
       <c r="E28" t="n">
         <v>0.8708</v>
@@ -998,10 +998,10 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.001937</v>
+        <v>0.0002671</v>
       </c>
       <c r="D29" t="n">
-        <v>5.772</v>
+        <v>5.768</v>
       </c>
       <c r="E29" t="n">
         <v>0.9781</v>
@@ -1018,10 +1018,10 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0002671</v>
+        <v>0.0001061</v>
       </c>
       <c r="D30" t="n">
-        <v>5.768</v>
+        <v>5.735</v>
       </c>
       <c r="E30" t="n">
         <v>1.092</v>
@@ -1038,10 +1038,10 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0001061</v>
+        <v>0.0002671</v>
       </c>
       <c r="D31" t="n">
-        <v>5.86</v>
+        <v>5.705</v>
       </c>
       <c r="E31" t="n">
         <v>0.8046</v>
@@ -1058,10 +1058,10 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0002671</v>
+        <v>0.0004712</v>
       </c>
       <c r="D32" t="n">
-        <v>5.846</v>
+        <v>5.723</v>
       </c>
       <c r="E32" t="n">
         <v>0.2972</v>
@@ -1078,10 +1078,10 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0004712</v>
+        <v>5.681e-06</v>
       </c>
       <c r="D33" t="n">
-        <v>5.749</v>
+        <v>5.772</v>
       </c>
       <c r="E33" t="n">
         <v>0.4281</v>
@@ -1098,10 +1098,10 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.02777</v>
+        <v>0.01732</v>
       </c>
       <c r="D34" t="n">
-        <v>5.092</v>
+        <v>4.946</v>
       </c>
       <c r="E34" t="n">
         <v>0.0883</v>
@@ -1118,10 +1118,10 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.001494</v>
+        <v>0.002922</v>
       </c>
       <c r="D35" t="n">
-        <v>5.901</v>
+        <v>5.832</v>
       </c>
       <c r="E35" t="n">
         <v>0.4095</v>
@@ -1138,10 +1138,10 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0.002922</v>
+        <v>0.0006306</v>
       </c>
       <c r="D36" t="n">
-        <v>6.127</v>
+        <v>6.133</v>
       </c>
       <c r="E36" t="n">
         <v>0.8233</v>
@@ -1158,10 +1158,10 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0006306</v>
+        <v>0.0001719</v>
       </c>
       <c r="D37" t="n">
-        <v>6.089</v>
+        <v>6.269</v>
       </c>
       <c r="E37" t="n">
         <v>0.6877</v>
@@ -1178,10 +1178,10 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0001719</v>
+        <v>0.001069</v>
       </c>
       <c r="D38" t="n">
-        <v>6.185</v>
+        <v>6.361</v>
       </c>
       <c r="E38" t="n">
         <v>0.476</v>
@@ -1198,10 +1198,10 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.001069</v>
+        <v>0.0002812</v>
       </c>
       <c r="D39" t="n">
-        <v>6.335</v>
+        <v>6.393</v>
       </c>
       <c r="E39" t="n">
         <v>0.4138</v>
@@ -1218,10 +1218,10 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0002812</v>
+        <v>0.0001461</v>
       </c>
       <c r="D40" t="n">
-        <v>6.341</v>
+        <v>6.374</v>
       </c>
       <c r="E40" t="n">
         <v>0.3649</v>
@@ -1238,10 +1238,10 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.02613</v>
+        <v>0.0286</v>
       </c>
       <c r="D41" t="n">
-        <v>5.043</v>
+        <v>5.206</v>
       </c>
       <c r="E41" t="n">
         <v>0.037</v>
@@ -1258,10 +1258,10 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>7.890999999999999e-06</v>
+        <v>0.000505</v>
       </c>
       <c r="D42" t="n">
-        <v>5.954</v>
+        <v>5.988</v>
       </c>
       <c r="E42" t="n">
         <v>0.6072</v>
@@ -1278,10 +1278,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4577</v>
+        <v>0.4081</v>
       </c>
       <c r="D43" t="n">
-        <v>5.047</v>
+        <v>4.755</v>
       </c>
       <c r="E43" t="n">
         <v>0.4592</v>
@@ -1298,10 +1298,10 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0002045</v>
+        <v>0.002354</v>
       </c>
       <c r="D44" t="n">
-        <v>6.582</v>
+        <v>6.054</v>
       </c>
       <c r="E44" t="n">
         <v>0.5487</v>
@@ -1318,10 +1318,10 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.002354</v>
+        <v>0.00129</v>
       </c>
       <c r="D45" t="n">
-        <v>6.634</v>
+        <v>6.508</v>
       </c>
       <c r="E45" t="n">
         <v>0.9028</v>
@@ -1338,10 +1338,10 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.00129</v>
+        <v>0.00479</v>
       </c>
       <c r="D46" t="n">
-        <v>6.625</v>
+        <v>6.827</v>
       </c>
       <c r="E46" t="n">
         <v>0.8683999999999999</v>
@@ -1358,10 +1358,10 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.00479</v>
+        <v>3.551e-05</v>
       </c>
       <c r="D47" t="n">
-        <v>6.751</v>
+        <v>7.108</v>
       </c>
       <c r="E47" t="n">
         <v>0.483</v>
@@ -1378,10 +1378,10 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>3.551e-05</v>
+        <v>8.609e-05</v>
       </c>
       <c r="D48" t="n">
-        <v>7.113</v>
+        <v>7.314</v>
       </c>
       <c r="E48" t="n">
         <v>0.5113</v>
@@ -1398,10 +1398,10 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>8.609e-05</v>
+        <v>0.001841</v>
       </c>
       <c r="D49" t="n">
-        <v>7.171</v>
+        <v>7.351</v>
       </c>
       <c r="E49" t="n">
         <v>0.6042</v>
@@ -1418,10 +1418,10 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1182</v>
+        <v>0.08749</v>
       </c>
       <c r="D50" t="n">
-        <v>5.289</v>
+        <v>5.858</v>
       </c>
       <c r="E50" t="n">
         <v>0.3804</v>
@@ -1438,10 +1438,10 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>1.403e-05</v>
+        <v>0.003351</v>
       </c>
       <c r="D51" t="n">
-        <v>6.289</v>
+        <v>6.655</v>
       </c>
       <c r="E51" t="n">
         <v>1.102</v>
@@ -1458,10 +1458,10 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>0.003351</v>
+        <v>0.0003045</v>
       </c>
       <c r="D52" t="n">
-        <v>6.51</v>
+        <v>6.531</v>
       </c>
       <c r="E52" t="n">
         <v>1.376</v>
@@ -1478,10 +1478,10 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0003045</v>
+        <v>0.001467</v>
       </c>
       <c r="D53" t="n">
-        <v>6.332</v>
+        <v>6.187</v>
       </c>
       <c r="E53" t="n">
         <v>1.739</v>
@@ -1498,10 +1498,10 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.001467</v>
+        <v>0.001435</v>
       </c>
       <c r="D54" t="n">
-        <v>6.269</v>
+        <v>5.854</v>
       </c>
       <c r="E54" t="n">
         <v>1.21</v>
@@ -1518,10 +1518,10 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.001435</v>
+        <v>0.003602</v>
       </c>
       <c r="D55" t="n">
-        <v>5.811</v>
+        <v>5.616</v>
       </c>
       <c r="E55" t="n">
         <v>0.9405</v>
@@ -1538,10 +1538,10 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.003602</v>
+        <v>0.002066</v>
       </c>
       <c r="D56" t="n">
-        <v>5.425</v>
+        <v>5.467</v>
       </c>
       <c r="E56" t="n">
         <v>1.215</v>
@@ -1558,10 +1558,10 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.002066</v>
+        <v>0.001003</v>
       </c>
       <c r="D57" t="n">
-        <v>5.557</v>
+        <v>5.405</v>
       </c>
       <c r="E57" t="n">
         <v>0.4551</v>
@@ -1578,10 +1578,10 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>0.001003</v>
+        <v>0.008064999999999999</v>
       </c>
       <c r="D58" t="n">
-        <v>5.238</v>
+        <v>5.353</v>
       </c>
       <c r="E58" t="n">
         <v>0.4266</v>
@@ -1598,10 +1598,10 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.008064999999999999</v>
+        <v>0.006485</v>
       </c>
       <c r="D59" t="n">
-        <v>5.144</v>
+        <v>5.253</v>
       </c>
       <c r="E59" t="n">
         <v>0.5847</v>
@@ -1618,10 +1618,10 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>0.006485</v>
+        <v>5.74e-05</v>
       </c>
       <c r="D60" t="n">
-        <v>5.281</v>
+        <v>5.161</v>
       </c>
       <c r="E60" t="n">
         <v>0.1414</v>
@@ -1638,10 +1638,10 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>0.2548</v>
+        <v>0.194</v>
       </c>
       <c r="D61" t="n">
-        <v>5.083</v>
+        <v>4.912</v>
       </c>
       <c r="E61" t="n">
         <v>0.191</v>
@@ -1658,10 +1658,10 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>0.02748</v>
+        <v>0.01743</v>
       </c>
       <c r="D62" t="n">
-        <v>4.555</v>
+        <v>4.294</v>
       </c>
       <c r="E62" t="n">
         <v>0.5453</v>
@@ -1678,10 +1678,10 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>0.001621</v>
+        <v>0.0003016</v>
       </c>
       <c r="D63" t="n">
-        <v>5.397</v>
+        <v>5.053</v>
       </c>
       <c r="E63" t="n">
         <v>1.361</v>
@@ -1698,10 +1698,10 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0003016</v>
+        <v>0.001136</v>
       </c>
       <c r="D64" t="n">
-        <v>5.459</v>
+        <v>5.389</v>
       </c>
       <c r="E64" t="n">
         <v>1.516</v>
@@ -1718,10 +1718,10 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.001136</v>
+        <v>0.004142</v>
       </c>
       <c r="D65" t="n">
-        <v>5.798</v>
+        <v>5.696</v>
       </c>
       <c r="E65" t="n">
         <v>1.697</v>
@@ -1738,10 +1738,10 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.004142</v>
+        <v>0.0009496</v>
       </c>
       <c r="D66" t="n">
-        <v>6.247</v>
+        <v>6.076</v>
       </c>
       <c r="E66" t="n">
         <v>2.258</v>
@@ -1758,10 +1758,10 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0009496</v>
+        <v>0.001266</v>
       </c>
       <c r="D67" t="n">
-        <v>6.376</v>
+        <v>6.466</v>
       </c>
       <c r="E67" t="n">
         <v>2.06</v>
@@ -1778,10 +1778,10 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.001266</v>
+        <v>0.002644</v>
       </c>
       <c r="D68" t="n">
-        <v>6.621</v>
+        <v>6.801</v>
       </c>
       <c r="E68" t="n">
         <v>1.491</v>
@@ -1798,10 +1798,10 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>0.002644</v>
+        <v>4.899e-06</v>
       </c>
       <c r="D69" t="n">
-        <v>6.99</v>
+        <v>7.114</v>
       </c>
       <c r="E69" t="n">
         <v>1.061</v>
@@ -1818,10 +1818,10 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>4.899e-06</v>
+        <v>0.0002169</v>
       </c>
       <c r="D70" t="n">
-        <v>7.357</v>
+        <v>7.399</v>
       </c>
       <c r="E70" t="n">
         <v>0.9724</v>
@@ -1838,10 +1838,10 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.0002169</v>
+        <v>0.000407</v>
       </c>
       <c r="D71" t="n">
-        <v>7.45</v>
+        <v>7.587</v>
       </c>
       <c r="E71" t="n">
         <v>0.3644</v>
@@ -1858,10 +1858,10 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>0.6113</v>
+        <v>0.4625</v>
       </c>
       <c r="D72" t="n">
-        <v>5.114</v>
+        <v>5.055</v>
       </c>
       <c r="E72" t="n">
         <v>0.1405</v>

</xml_diff>

<commit_message>
Updated on 04-30-2024 at 22:19
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -458,13 +458,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07140000000000001</v>
+        <v>2.473e-19</v>
       </c>
       <c r="D2" t="n">
-        <v>1.246</v>
+        <v>2.429</v>
       </c>
       <c r="E2" t="n">
-        <v>2.38</v>
+        <v>1.715</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
@@ -478,13 +478,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0346</v>
+        <v>1.81e-18</v>
       </c>
       <c r="D3" t="n">
-        <v>1.711</v>
+        <v>2.248</v>
       </c>
       <c r="E3" t="n">
-        <v>1.819</v>
+        <v>0.6059</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>
@@ -498,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0005845</v>
+        <v>5.073e-18</v>
       </c>
       <c r="D4" t="n">
-        <v>2.071</v>
+        <v>3.451</v>
       </c>
       <c r="E4" t="n">
-        <v>1.742</v>
+        <v>0.8223</v>
       </c>
       <c r="F4" t="n">
         <v>5</v>
@@ -518,13 +518,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.008944000000000001</v>
+        <v>6.555e-19</v>
       </c>
       <c r="D5" t="n">
-        <v>2.283</v>
+        <v>2.633</v>
       </c>
       <c r="E5" t="n">
-        <v>1.121</v>
+        <v>0.1534</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
@@ -538,13 +538,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.002097</v>
+        <v>1.301e-18</v>
       </c>
       <c r="D6" t="n">
-        <v>2.467</v>
+        <v>2.951</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4541</v>
+        <v>0.1706</v>
       </c>
       <c r="F6" t="n">
         <v>5</v>
@@ -558,16 +558,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>4.872e-05</v>
+        <v>0.351</v>
       </c>
       <c r="D7" t="n">
-        <v>2.63</v>
+        <v>1.446</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9320000000000001</v>
+        <v>0.4955</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -578,13 +578,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.006281</v>
+        <v>3.792e-17</v>
       </c>
       <c r="D8" t="n">
-        <v>2.677</v>
+        <v>3.122</v>
       </c>
       <c r="E8" t="n">
-        <v>1.225</v>
+        <v>2.671</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
@@ -598,13 +598,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.04933</v>
+        <v>9.334e-18</v>
       </c>
       <c r="D9" t="n">
-        <v>2.71</v>
+        <v>5.336</v>
       </c>
       <c r="E9" t="n">
-        <v>1.321</v>
+        <v>2.182</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>
@@ -618,13 +618,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.04533</v>
+        <v>4.402e-18</v>
       </c>
       <c r="D10" t="n">
-        <v>2.742</v>
+        <v>3.549</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9503</v>
+        <v>0.5923</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -638,16 +638,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.001937</v>
+        <v>0.09017</v>
       </c>
       <c r="D11" t="n">
-        <v>2.781</v>
+        <v>2.41</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8944</v>
+        <v>0.1071</v>
       </c>
       <c r="F11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -658,13 +658,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.001944</v>
+        <v>6.26e-19</v>
       </c>
       <c r="D12" t="n">
-        <v>2.792</v>
+        <v>3.238</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6382</v>
+        <v>0.7953</v>
       </c>
       <c r="F12" t="n">
         <v>5</v>
@@ -678,13 +678,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0006522</v>
+        <v>2.761e-19</v>
       </c>
       <c r="D13" t="n">
-        <v>2.94</v>
+        <v>3.334</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5722</v>
+        <v>0.9553</v>
       </c>
       <c r="F13" t="n">
         <v>5</v>
@@ -698,16 +698,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2507</v>
+        <v>3.738e-18</v>
       </c>
       <c r="D14" t="n">
-        <v>2.227</v>
+        <v>3.952</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2538</v>
+        <v>1.361</v>
       </c>
       <c r="F14" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -718,16 +718,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1076</v>
+        <v>5.053e-18</v>
       </c>
       <c r="D15" t="n">
-        <v>2.284</v>
+        <v>4.032</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2041</v>
+        <v>1.121</v>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -738,13 +738,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>4.638e-07</v>
+        <v>4.052e-18</v>
       </c>
       <c r="D16" t="n">
-        <v>3.349</v>
+        <v>4.107</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4351</v>
+        <v>1.278</v>
       </c>
       <c r="F16" t="n">
         <v>5</v>
@@ -758,13 +758,13 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>8.296000000000001e-05</v>
+        <v>4.711e-18</v>
       </c>
       <c r="D17" t="n">
-        <v>3.802</v>
+        <v>4.491</v>
       </c>
       <c r="E17" t="n">
-        <v>0.844</v>
+        <v>1.675</v>
       </c>
       <c r="F17" t="n">
         <v>5</v>
@@ -778,13 +778,13 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0003701</v>
+        <v>2.61e-19</v>
       </c>
       <c r="D18" t="n">
-        <v>4.139</v>
+        <v>4.287</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9012</v>
+        <v>0.9827</v>
       </c>
       <c r="F18" t="n">
         <v>5</v>
@@ -798,16 +798,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.008718999999999999</v>
+        <v>0.003197</v>
       </c>
       <c r="D19" t="n">
-        <v>3.081</v>
+        <v>3.884</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5685</v>
+        <v>0.2202</v>
       </c>
       <c r="F19" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -818,13 +818,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0006609</v>
+        <v>1.423e-17</v>
       </c>
       <c r="D20" t="n">
-        <v>4.45</v>
+        <v>6.008</v>
       </c>
       <c r="E20" t="n">
-        <v>1.179</v>
+        <v>0.2463</v>
       </c>
       <c r="F20" t="n">
         <v>5</v>
@@ -838,13 +838,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.007643</v>
+        <v>1.188e-18</v>
       </c>
       <c r="D21" t="n">
-        <v>4.945</v>
+        <v>5.064</v>
       </c>
       <c r="E21" t="n">
-        <v>1.323</v>
+        <v>0.3729</v>
       </c>
       <c r="F21" t="n">
         <v>5</v>
@@ -858,13 +858,13 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.003798</v>
+        <v>3.725e-19</v>
       </c>
       <c r="D22" t="n">
-        <v>5.237</v>
+        <v>5.486</v>
       </c>
       <c r="E22" t="n">
-        <v>1.304</v>
+        <v>0.3875</v>
       </c>
       <c r="F22" t="n">
         <v>5</v>
@@ -878,13 +878,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0002045</v>
+        <v>2.309e-19</v>
       </c>
       <c r="D23" t="n">
-        <v>5.45</v>
+        <v>5.572</v>
       </c>
       <c r="E23" t="n">
-        <v>0.7727000000000001</v>
+        <v>0.4257</v>
       </c>
       <c r="F23" t="n">
         <v>5</v>
@@ -898,13 +898,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0006052</v>
+        <v>5.297e-19</v>
       </c>
       <c r="D24" t="n">
-        <v>5.654</v>
+        <v>6.303</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5427</v>
+        <v>0.6127</v>
       </c>
       <c r="F24" t="n">
         <v>5</v>
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.02814</v>
+        <v>5.022e-20</v>
       </c>
       <c r="D25" t="n">
-        <v>4.409</v>
+        <v>5.954</v>
       </c>
       <c r="E25" t="n">
-        <v>0.05253</v>
+        <v>0.841</v>
       </c>
       <c r="F25" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -938,16 +938,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.04602</v>
+        <v>0.001364</v>
       </c>
       <c r="D26" t="n">
-        <v>4.106</v>
+        <v>4.536</v>
       </c>
       <c r="E26" t="n">
-        <v>0.146</v>
+        <v>0.3336</v>
       </c>
       <c r="F26" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
@@ -958,13 +958,13 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.00139</v>
+        <v>1.771e-18</v>
       </c>
       <c r="D27" t="n">
-        <v>5.493</v>
+        <v>5.316</v>
       </c>
       <c r="E27" t="n">
-        <v>0.4769</v>
+        <v>0.5809</v>
       </c>
       <c r="F27" t="n">
         <v>5</v>
@@ -978,13 +978,13 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.001937</v>
+        <v>4.031e-19</v>
       </c>
       <c r="D28" t="n">
-        <v>5.754</v>
+        <v>6.067</v>
       </c>
       <c r="E28" t="n">
-        <v>0.8708</v>
+        <v>0.7125</v>
       </c>
       <c r="F28" t="n">
         <v>5</v>
@@ -998,13 +998,13 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0002671</v>
+        <v>4.213e-21</v>
       </c>
       <c r="D29" t="n">
-        <v>5.768</v>
+        <v>6.252</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9781</v>
+        <v>0.4791</v>
       </c>
       <c r="F29" t="n">
         <v>5</v>
@@ -1018,13 +1018,13 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0001061</v>
+        <v>2.488e-21</v>
       </c>
       <c r="D30" t="n">
-        <v>5.735</v>
+        <v>6.048</v>
       </c>
       <c r="E30" t="n">
-        <v>1.092</v>
+        <v>0.3386</v>
       </c>
       <c r="F30" t="n">
         <v>5</v>
@@ -1038,16 +1038,16 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0002671</v>
+        <v>0.0002918</v>
       </c>
       <c r="D31" t="n">
-        <v>5.705</v>
+        <v>5.026</v>
       </c>
       <c r="E31" t="n">
-        <v>0.8046</v>
+        <v>0.253</v>
       </c>
       <c r="F31" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
@@ -1058,13 +1058,13 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0004712</v>
+        <v>6.51e-19</v>
       </c>
       <c r="D32" t="n">
-        <v>5.723</v>
+        <v>5.849</v>
       </c>
       <c r="E32" t="n">
-        <v>0.2972</v>
+        <v>0.922</v>
       </c>
       <c r="F32" t="n">
         <v>5</v>
@@ -1078,13 +1078,13 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>5.681e-06</v>
+        <v>5.907000000000001e-20</v>
       </c>
       <c r="D33" t="n">
-        <v>5.772</v>
+        <v>5.812</v>
       </c>
       <c r="E33" t="n">
-        <v>0.4281</v>
+        <v>0.7369</v>
       </c>
       <c r="F33" t="n">
         <v>5</v>
@@ -1098,16 +1098,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01732</v>
+        <v>4.038e-18</v>
       </c>
       <c r="D34" t="n">
-        <v>4.946</v>
+        <v>6.829</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0883</v>
+        <v>0.9738</v>
       </c>
       <c r="F34" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -1118,13 +1118,13 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.002922</v>
+        <v>1.077e-18</v>
       </c>
       <c r="D35" t="n">
-        <v>5.832</v>
+        <v>6.376</v>
       </c>
       <c r="E35" t="n">
-        <v>0.4095</v>
+        <v>1.074</v>
       </c>
       <c r="F35" t="n">
         <v>5</v>
@@ -1138,13 +1138,13 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0006306</v>
+        <v>4.016e-19</v>
       </c>
       <c r="D36" t="n">
-        <v>6.133</v>
+        <v>6.471</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8233</v>
+        <v>1.065</v>
       </c>
       <c r="F36" t="n">
         <v>5</v>
@@ -1158,13 +1158,13 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0001719</v>
+        <v>1.252e-18</v>
       </c>
       <c r="D37" t="n">
-        <v>6.269</v>
+        <v>6.166</v>
       </c>
       <c r="E37" t="n">
-        <v>0.6877</v>
+        <v>0.2847</v>
       </c>
       <c r="F37" t="n">
         <v>5</v>
@@ -1178,13 +1178,13 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.001069</v>
+        <v>2.446e-19</v>
       </c>
       <c r="D38" t="n">
-        <v>6.361</v>
+        <v>6.72</v>
       </c>
       <c r="E38" t="n">
-        <v>0.476</v>
+        <v>0.4637</v>
       </c>
       <c r="F38" t="n">
         <v>5</v>
@@ -1198,13 +1198,13 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0002812</v>
+        <v>4.01e-21</v>
       </c>
       <c r="D39" t="n">
-        <v>6.393</v>
+        <v>6.863</v>
       </c>
       <c r="E39" t="n">
-        <v>0.4138</v>
+        <v>0.7395</v>
       </c>
       <c r="F39" t="n">
         <v>5</v>
@@ -1218,13 +1218,13 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0001461</v>
+        <v>1.722e-19</v>
       </c>
       <c r="D40" t="n">
-        <v>6.374</v>
+        <v>6.569</v>
       </c>
       <c r="E40" t="n">
-        <v>0.3649</v>
+        <v>0.8516</v>
       </c>
       <c r="F40" t="n">
         <v>5</v>
@@ -1238,16 +1238,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0286</v>
+        <v>1.741e-18</v>
       </c>
       <c r="D41" t="n">
-        <v>5.206</v>
+        <v>6.26</v>
       </c>
       <c r="E41" t="n">
-        <v>0.037</v>
+        <v>1.042</v>
       </c>
       <c r="F41" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -1258,13 +1258,13 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.000505</v>
+        <v>1.384e-19</v>
       </c>
       <c r="D42" t="n">
-        <v>5.988</v>
+        <v>6.623</v>
       </c>
       <c r="E42" t="n">
-        <v>0.6072</v>
+        <v>1.246</v>
       </c>
       <c r="F42" t="n">
         <v>5</v>
@@ -1278,16 +1278,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4081</v>
+        <v>0.06199</v>
       </c>
       <c r="D43" t="n">
-        <v>4.755</v>
+        <v>4.316</v>
       </c>
       <c r="E43" t="n">
-        <v>0.4592</v>
+        <v>0.2819</v>
       </c>
       <c r="F43" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
@@ -1298,13 +1298,13 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.002354</v>
+        <v>2.274e-17</v>
       </c>
       <c r="D44" t="n">
-        <v>6.054</v>
+        <v>6.905</v>
       </c>
       <c r="E44" t="n">
-        <v>0.5487</v>
+        <v>1.989</v>
       </c>
       <c r="F44" t="n">
         <v>5</v>
@@ -1318,13 +1318,13 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.00129</v>
+        <v>6.644e-19</v>
       </c>
       <c r="D45" t="n">
-        <v>6.508</v>
+        <v>6.15</v>
       </c>
       <c r="E45" t="n">
-        <v>0.9028</v>
+        <v>2.506</v>
       </c>
       <c r="F45" t="n">
         <v>5</v>
@@ -1338,13 +1338,13 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.00479</v>
+        <v>1.535e-19</v>
       </c>
       <c r="D46" t="n">
-        <v>6.827</v>
+        <v>6.803</v>
       </c>
       <c r="E46" t="n">
-        <v>0.8683999999999999</v>
+        <v>2.1</v>
       </c>
       <c r="F46" t="n">
         <v>5</v>
@@ -1358,13 +1358,13 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>3.551e-05</v>
+        <v>8.204e-19</v>
       </c>
       <c r="D47" t="n">
-        <v>7.108</v>
+        <v>7.293</v>
       </c>
       <c r="E47" t="n">
-        <v>0.483</v>
+        <v>0.8519</v>
       </c>
       <c r="F47" t="n">
         <v>5</v>
@@ -1378,16 +1378,16 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>8.609e-05</v>
+        <v>0.406</v>
       </c>
       <c r="D48" t="n">
-        <v>7.314</v>
+        <v>6.291</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5113</v>
+        <v>0.144</v>
       </c>
       <c r="F48" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49">
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.001841</v>
+        <v>0.003674</v>
       </c>
       <c r="D49" t="n">
-        <v>7.351</v>
+        <v>5.464</v>
       </c>
       <c r="E49" t="n">
-        <v>0.6042</v>
+        <v>0.7191</v>
       </c>
       <c r="F49" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50">
@@ -1418,16 +1418,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.08749</v>
+        <v>2.14e-17</v>
       </c>
       <c r="D50" t="n">
-        <v>5.858</v>
+        <v>5.941</v>
       </c>
       <c r="E50" t="n">
-        <v>0.3804</v>
+        <v>2.329</v>
       </c>
       <c r="F50" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
@@ -1438,13 +1438,13 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>0.003351</v>
+        <v>1.261e-17</v>
       </c>
       <c r="D51" t="n">
-        <v>6.655</v>
+        <v>6.84</v>
       </c>
       <c r="E51" t="n">
-        <v>1.102</v>
+        <v>3.537</v>
       </c>
       <c r="F51" t="n">
         <v>5</v>
@@ -1458,13 +1458,13 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0003045</v>
+        <v>1.349e-18</v>
       </c>
       <c r="D52" t="n">
-        <v>6.531</v>
+        <v>7.2</v>
       </c>
       <c r="E52" t="n">
-        <v>1.376</v>
+        <v>3.006</v>
       </c>
       <c r="F52" t="n">
         <v>5</v>
@@ -1478,13 +1478,13 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>0.001467</v>
+        <v>1.237e-18</v>
       </c>
       <c r="D53" t="n">
-        <v>6.187</v>
+        <v>6.375</v>
       </c>
       <c r="E53" t="n">
-        <v>1.739</v>
+        <v>2.212</v>
       </c>
       <c r="F53" t="n">
         <v>5</v>
@@ -1498,13 +1498,13 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.001435</v>
+        <v>1.935e-18</v>
       </c>
       <c r="D54" t="n">
-        <v>5.854</v>
+        <v>6.707</v>
       </c>
       <c r="E54" t="n">
-        <v>1.21</v>
+        <v>0.4235</v>
       </c>
       <c r="F54" t="n">
         <v>5</v>
@@ -1518,13 +1518,13 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.003602</v>
+        <v>5.889e-19</v>
       </c>
       <c r="D55" t="n">
-        <v>5.616</v>
+        <v>5.466</v>
       </c>
       <c r="E55" t="n">
-        <v>0.9405</v>
+        <v>1.096</v>
       </c>
       <c r="F55" t="n">
         <v>5</v>
@@ -1538,13 +1538,13 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.002066</v>
+        <v>2.337e-18</v>
       </c>
       <c r="D56" t="n">
-        <v>5.467</v>
+        <v>5.359</v>
       </c>
       <c r="E56" t="n">
-        <v>1.215</v>
+        <v>1.331</v>
       </c>
       <c r="F56" t="n">
         <v>5</v>
@@ -1558,13 +1558,13 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.001003</v>
+        <v>2.15e-18</v>
       </c>
       <c r="D57" t="n">
-        <v>5.405</v>
+        <v>6.439</v>
       </c>
       <c r="E57" t="n">
-        <v>0.4551</v>
+        <v>1.968</v>
       </c>
       <c r="F57" t="n">
         <v>5</v>
@@ -1578,13 +1578,13 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>0.008064999999999999</v>
+        <v>3.592e-18</v>
       </c>
       <c r="D58" t="n">
-        <v>5.353</v>
+        <v>4.914</v>
       </c>
       <c r="E58" t="n">
-        <v>0.4266</v>
+        <v>1.268</v>
       </c>
       <c r="F58" t="n">
         <v>5</v>
@@ -1598,13 +1598,13 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.006485</v>
+        <v>1.538e-18</v>
       </c>
       <c r="D59" t="n">
-        <v>5.253</v>
+        <v>5.414</v>
       </c>
       <c r="E59" t="n">
-        <v>0.5847</v>
+        <v>0.3571</v>
       </c>
       <c r="F59" t="n">
         <v>5</v>
@@ -1618,13 +1618,13 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>5.74e-05</v>
+        <v>8.575e-19</v>
       </c>
       <c r="D60" t="n">
-        <v>5.161</v>
+        <v>6.023</v>
       </c>
       <c r="E60" t="n">
-        <v>0.1414</v>
+        <v>0.2395</v>
       </c>
       <c r="F60" t="n">
         <v>5</v>
@@ -1641,13 +1641,13 @@
         <v>0.194</v>
       </c>
       <c r="D61" t="n">
-        <v>4.912</v>
+        <v>6.576</v>
       </c>
       <c r="E61" t="n">
-        <v>0.191</v>
+        <v>0.1818</v>
       </c>
       <c r="F61" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62">
@@ -1658,16 +1658,16 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>0.01743</v>
+        <v>0.147</v>
       </c>
       <c r="D62" t="n">
-        <v>4.294</v>
+        <v>6.771</v>
       </c>
       <c r="E62" t="n">
-        <v>0.5453</v>
+        <v>0.1987</v>
       </c>
       <c r="F62" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63">
@@ -1678,13 +1678,13 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>0.0003016</v>
+        <v>1.016e-17</v>
       </c>
       <c r="D63" t="n">
-        <v>5.053</v>
+        <v>6.383</v>
       </c>
       <c r="E63" t="n">
-        <v>1.361</v>
+        <v>0.9268999999999999</v>
       </c>
       <c r="F63" t="n">
         <v>5</v>
@@ -1698,13 +1698,13 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>0.001136</v>
+        <v>8.577e-19</v>
       </c>
       <c r="D64" t="n">
-        <v>5.389</v>
+        <v>5.523</v>
       </c>
       <c r="E64" t="n">
-        <v>1.516</v>
+        <v>1.142</v>
       </c>
       <c r="F64" t="n">
         <v>5</v>
@@ -1718,13 +1718,13 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.004142</v>
+        <v>6.728e-18</v>
       </c>
       <c r="D65" t="n">
-        <v>5.696</v>
+        <v>6.621</v>
       </c>
       <c r="E65" t="n">
-        <v>1.697</v>
+        <v>1.437</v>
       </c>
       <c r="F65" t="n">
         <v>5</v>
@@ -1738,13 +1738,13 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.0009496</v>
+        <v>1.294e-17</v>
       </c>
       <c r="D66" t="n">
-        <v>6.076</v>
+        <v>7.142</v>
       </c>
       <c r="E66" t="n">
-        <v>2.258</v>
+        <v>2.165</v>
       </c>
       <c r="F66" t="n">
         <v>5</v>
@@ -1758,13 +1758,13 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>0.001266</v>
+        <v>7.243e-19</v>
       </c>
       <c r="D67" t="n">
-        <v>6.466</v>
+        <v>6.465</v>
       </c>
       <c r="E67" t="n">
-        <v>2.06</v>
+        <v>1.611</v>
       </c>
       <c r="F67" t="n">
         <v>5</v>
@@ -1778,13 +1778,13 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.002644</v>
+        <v>2.539e-19</v>
       </c>
       <c r="D68" t="n">
-        <v>6.801</v>
+        <v>7.099</v>
       </c>
       <c r="E68" t="n">
-        <v>1.491</v>
+        <v>0.5243</v>
       </c>
       <c r="F68" t="n">
         <v>5</v>
@@ -1798,16 +1798,16 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>4.899e-06</v>
+        <v>0.006925</v>
       </c>
       <c r="D69" t="n">
-        <v>7.114</v>
+        <v>4.937</v>
       </c>
       <c r="E69" t="n">
-        <v>1.061</v>
+        <v>0.2123</v>
       </c>
       <c r="F69" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
@@ -1818,16 +1818,16 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.0002169</v>
+        <v>0.0007808</v>
       </c>
       <c r="D70" t="n">
-        <v>7.399</v>
+        <v>4.815</v>
       </c>
       <c r="E70" t="n">
-        <v>0.9724</v>
+        <v>0.3495</v>
       </c>
       <c r="F70" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71">
@@ -1838,13 +1838,13 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.000407</v>
+        <v>1.359e-19</v>
       </c>
       <c r="D71" t="n">
-        <v>7.587</v>
+        <v>6.906</v>
       </c>
       <c r="E71" t="n">
-        <v>0.3644</v>
+        <v>1.134</v>
       </c>
       <c r="F71" t="n">
         <v>5</v>
@@ -1858,16 +1858,16 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>0.4625</v>
+        <v>7.207e-19</v>
       </c>
       <c r="D72" t="n">
-        <v>5.055</v>
+        <v>8.228</v>
       </c>
       <c r="E72" t="n">
-        <v>0.1405</v>
+        <v>0.9114</v>
       </c>
       <c r="F72" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 05-01-2024 at 13:53
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -458,16 +458,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>2.473e-19</v>
+        <v>0.5547</v>
       </c>
       <c r="D2" t="n">
-        <v>2.429</v>
+        <v>1.091</v>
       </c>
       <c r="E2" t="n">
-        <v>1.715</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1.81e-18</v>
+        <v>0.7871</v>
       </c>
       <c r="D3" t="n">
-        <v>2.248</v>
+        <v>1.041</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6059</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -498,16 +498,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>5.073e-18</v>
+        <v>0.6943</v>
       </c>
       <c r="D4" t="n">
-        <v>3.451</v>
+        <v>1.125</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8223</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -518,16 +518,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>6.555e-19</v>
+        <v>0.6021</v>
       </c>
       <c r="D5" t="n">
-        <v>2.633</v>
+        <v>1.216</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1534</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.301e-18</v>
+        <v>0.4131</v>
       </c>
       <c r="D6" t="n">
-        <v>2.951</v>
+        <v>1.253</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1706</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -561,13 +561,13 @@
         <v>0.351</v>
       </c>
       <c r="D7" t="n">
-        <v>1.446</v>
+        <v>1.352</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4955</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -578,16 +578,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>3.792e-17</v>
+        <v>1.092</v>
       </c>
       <c r="D8" t="n">
-        <v>3.122</v>
+        <v>1.095</v>
       </c>
       <c r="E8" t="n">
-        <v>2.671</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>9.334e-18</v>
+        <v>0.1939</v>
       </c>
       <c r="D9" t="n">
-        <v>5.336</v>
+        <v>1.63</v>
       </c>
       <c r="E9" t="n">
-        <v>2.182</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -618,16 +618,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>4.402e-18</v>
+        <v>0.6674</v>
       </c>
       <c r="D10" t="n">
-        <v>3.549</v>
+        <v>1.492</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5923</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -638,16 +638,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.09017</v>
+        <v>0.4228</v>
       </c>
       <c r="D11" t="n">
-        <v>2.41</v>
+        <v>1.817</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1071</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -658,16 +658,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>6.26e-19</v>
+        <v>0.7419</v>
       </c>
       <c r="D12" t="n">
-        <v>3.238</v>
+        <v>1.594</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7953</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -678,16 +678,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>2.761e-19</v>
+        <v>0.7859</v>
       </c>
       <c r="D13" t="n">
-        <v>3.334</v>
+        <v>1.654</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9553</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
@@ -698,16 +698,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>3.738e-18</v>
+        <v>0.8205</v>
       </c>
       <c r="D14" t="n">
-        <v>3.952</v>
+        <v>1.797</v>
       </c>
       <c r="E14" t="n">
-        <v>1.361</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -718,16 +718,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>5.053e-18</v>
+        <v>1.012</v>
       </c>
       <c r="D15" t="n">
-        <v>4.032</v>
+        <v>1.534</v>
       </c>
       <c r="E15" t="n">
-        <v>1.121</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -738,16 +738,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>4.052e-18</v>
+        <v>0.1007</v>
       </c>
       <c r="D16" t="n">
-        <v>4.107</v>
+        <v>2.327</v>
       </c>
       <c r="E16" t="n">
-        <v>1.278</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -758,13 +758,13 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>4.711e-18</v>
+        <v>8.296000000000001e-05</v>
       </c>
       <c r="D17" t="n">
-        <v>4.491</v>
+        <v>3.598</v>
       </c>
       <c r="E17" t="n">
-        <v>1.675</v>
+        <v>0.3733</v>
       </c>
       <c r="F17" t="n">
         <v>5</v>
@@ -778,16 +778,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>2.61e-19</v>
+        <v>0.02765</v>
       </c>
       <c r="D18" t="n">
-        <v>4.287</v>
+        <v>2.838</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9827</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -798,13 +798,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.003197</v>
+        <v>0.1738</v>
       </c>
       <c r="D19" t="n">
-        <v>3.884</v>
+        <v>2.872</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2202</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
         <v>15</v>
@@ -818,16 +818,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>1.423e-17</v>
+        <v>0.03501</v>
       </c>
       <c r="D20" t="n">
-        <v>6.008</v>
+        <v>3.167</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2463</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -838,16 +838,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>1.188e-18</v>
+        <v>0.1341</v>
       </c>
       <c r="D21" t="n">
-        <v>5.064</v>
+        <v>3.207</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3729</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
@@ -858,16 +858,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>3.725e-19</v>
+        <v>0.05612</v>
       </c>
       <c r="D22" t="n">
-        <v>5.486</v>
+        <v>3.342</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3875</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
@@ -878,16 +878,16 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>2.309e-19</v>
+        <v>0.262</v>
       </c>
       <c r="D23" t="n">
-        <v>5.572</v>
+        <v>3.172</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4257</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
@@ -898,16 +898,16 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>5.297e-19</v>
+        <v>0.1853</v>
       </c>
       <c r="D24" t="n">
-        <v>6.303</v>
+        <v>3.307</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6127</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5.022e-20</v>
+        <v>0.5451</v>
       </c>
       <c r="D25" t="n">
-        <v>5.954</v>
+        <v>2.916</v>
       </c>
       <c r="E25" t="n">
-        <v>0.841</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
@@ -938,16 +938,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.001364</v>
+        <v>0.0008876999999999999</v>
       </c>
       <c r="D26" t="n">
-        <v>4.536</v>
+        <v>5.263</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3336</v>
+        <v>0.1375</v>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -958,16 +958,16 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>1.771e-18</v>
+        <v>0.02503</v>
       </c>
       <c r="D27" t="n">
-        <v>5.316</v>
+        <v>4.589</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5809</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -978,16 +978,16 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>4.031e-19</v>
+        <v>0.01462</v>
       </c>
       <c r="D28" t="n">
-        <v>6.067</v>
+        <v>4.589</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7125</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
@@ -998,16 +998,16 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>4.213e-21</v>
+        <v>0.0077</v>
       </c>
       <c r="D29" t="n">
-        <v>6.252</v>
+        <v>4.657</v>
       </c>
       <c r="E29" t="n">
-        <v>0.4791</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
@@ -1018,13 +1018,13 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>2.488e-21</v>
+        <v>0.0001061</v>
       </c>
       <c r="D30" t="n">
-        <v>6.048</v>
+        <v>5.513</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3386</v>
+        <v>0.07238</v>
       </c>
       <c r="F30" t="n">
         <v>5</v>
@@ -1038,16 +1038,16 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0002918</v>
+        <v>0.06807000000000001</v>
       </c>
       <c r="D31" t="n">
-        <v>5.026</v>
+        <v>4.737</v>
       </c>
       <c r="E31" t="n">
-        <v>0.253</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32">
@@ -1058,16 +1058,16 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>6.51e-19</v>
+        <v>0.143</v>
       </c>
       <c r="D32" t="n">
-        <v>5.849</v>
+        <v>4.348</v>
       </c>
       <c r="E32" t="n">
-        <v>0.922</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
@@ -1078,16 +1078,16 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>5.907000000000001e-20</v>
+        <v>0.1074</v>
       </c>
       <c r="D33" t="n">
-        <v>5.812</v>
+        <v>4.427</v>
       </c>
       <c r="E33" t="n">
-        <v>0.7369</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34">
@@ -1098,16 +1098,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>4.038e-18</v>
+        <v>0.4929</v>
       </c>
       <c r="D34" t="n">
-        <v>6.829</v>
+        <v>3.961</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9738</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
@@ -1118,16 +1118,16 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>1.077e-18</v>
+        <v>0.3971</v>
       </c>
       <c r="D35" t="n">
-        <v>6.376</v>
+        <v>4.047</v>
       </c>
       <c r="E35" t="n">
-        <v>1.074</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36">
@@ -1138,16 +1138,16 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>4.016e-19</v>
+        <v>0.005569</v>
       </c>
       <c r="D36" t="n">
-        <v>6.471</v>
+        <v>4.771</v>
       </c>
       <c r="E36" t="n">
-        <v>1.065</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
@@ -1158,16 +1158,16 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>1.252e-18</v>
+        <v>0.07881000000000001</v>
       </c>
       <c r="D37" t="n">
-        <v>6.166</v>
+        <v>4.998</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2847</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -1178,13 +1178,13 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>2.446e-19</v>
+        <v>0.001069</v>
       </c>
       <c r="D38" t="n">
-        <v>6.72</v>
+        <v>6.106</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4637</v>
+        <v>0.1564</v>
       </c>
       <c r="F38" t="n">
         <v>5</v>
@@ -1198,16 +1198,16 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>4.01e-21</v>
+        <v>0.2017</v>
       </c>
       <c r="D39" t="n">
-        <v>6.863</v>
+        <v>4.984</v>
       </c>
       <c r="E39" t="n">
-        <v>0.7395</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40">
@@ -1218,16 +1218,16 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>1.722e-19</v>
+        <v>0.1572</v>
       </c>
       <c r="D40" t="n">
-        <v>6.569</v>
+        <v>4.968</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8516</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41">
@@ -1238,16 +1238,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>1.741e-18</v>
+        <v>0.4605</v>
       </c>
       <c r="D41" t="n">
-        <v>6.26</v>
+        <v>4.586</v>
       </c>
       <c r="E41" t="n">
-        <v>1.042</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
@@ -1258,16 +1258,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>1.384e-19</v>
+        <v>0.006423</v>
       </c>
       <c r="D42" t="n">
-        <v>6.623</v>
+        <v>5.057</v>
       </c>
       <c r="E42" t="n">
-        <v>1.246</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
@@ -1278,16 +1278,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.06199</v>
+        <v>0.1434</v>
       </c>
       <c r="D43" t="n">
-        <v>4.316</v>
+        <v>5.187</v>
       </c>
       <c r="E43" t="n">
-        <v>0.2819</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44">
@@ -1298,16 +1298,16 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>2.274e-17</v>
+        <v>0.6493</v>
       </c>
       <c r="D44" t="n">
-        <v>6.905</v>
+        <v>4.823</v>
       </c>
       <c r="E44" t="n">
-        <v>1.989</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45">
@@ -1318,16 +1318,16 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>6.644e-19</v>
+        <v>0.6409</v>
       </c>
       <c r="D45" t="n">
-        <v>6.15</v>
+        <v>4.865</v>
       </c>
       <c r="E45" t="n">
-        <v>2.506</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46">
@@ -1338,16 +1338,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>1.535e-19</v>
+        <v>0.1509</v>
       </c>
       <c r="D46" t="n">
-        <v>6.803</v>
+        <v>5.343</v>
       </c>
       <c r="E46" t="n">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47">
@@ -1358,16 +1358,16 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>8.204e-19</v>
+        <v>0.5592</v>
       </c>
       <c r="D47" t="n">
-        <v>7.293</v>
+        <v>4.956</v>
       </c>
       <c r="E47" t="n">
-        <v>0.8519</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48">
@@ -1381,13 +1381,13 @@
         <v>0.406</v>
       </c>
       <c r="D48" t="n">
-        <v>6.291</v>
+        <v>5.559</v>
       </c>
       <c r="E48" t="n">
-        <v>0.144</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49">
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.003674</v>
+        <v>0.6852</v>
       </c>
       <c r="D49" t="n">
-        <v>5.464</v>
+        <v>5.047</v>
       </c>
       <c r="E49" t="n">
-        <v>0.7191</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50">
@@ -1418,16 +1418,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>2.14e-17</v>
+        <v>1.08</v>
       </c>
       <c r="D50" t="n">
-        <v>5.941</v>
+        <v>5.027</v>
       </c>
       <c r="E50" t="n">
-        <v>2.329</v>
+        <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
@@ -1438,13 +1438,13 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>1.261e-17</v>
+        <v>0.003351</v>
       </c>
       <c r="D51" t="n">
-        <v>6.84</v>
+        <v>6.489</v>
       </c>
       <c r="E51" t="n">
-        <v>3.537</v>
+        <v>0.6151</v>
       </c>
       <c r="F51" t="n">
         <v>5</v>
@@ -1458,16 +1458,16 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>1.349e-18</v>
+        <v>0.04785</v>
       </c>
       <c r="D52" t="n">
-        <v>7.2</v>
+        <v>5.734</v>
       </c>
       <c r="E52" t="n">
-        <v>3.006</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53">
@@ -1478,16 +1478,16 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>1.237e-18</v>
+        <v>0.05953</v>
       </c>
       <c r="D53" t="n">
-        <v>6.375</v>
+        <v>5.575</v>
       </c>
       <c r="E53" t="n">
-        <v>2.212</v>
+        <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54">
@@ -1498,16 +1498,16 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>1.935e-18</v>
+        <v>0.6843</v>
       </c>
       <c r="D54" t="n">
-        <v>6.707</v>
+        <v>5.541</v>
       </c>
       <c r="E54" t="n">
-        <v>0.4235</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55">
@@ -1518,16 +1518,16 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>5.889e-19</v>
+        <v>1.42</v>
       </c>
       <c r="D55" t="n">
-        <v>5.466</v>
+        <v>5.093</v>
       </c>
       <c r="E55" t="n">
-        <v>1.096</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56">
@@ -1538,16 +1538,16 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>2.337e-18</v>
+        <v>1.354</v>
       </c>
       <c r="D56" t="n">
-        <v>5.359</v>
+        <v>5.316</v>
       </c>
       <c r="E56" t="n">
-        <v>1.331</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57">
@@ -1558,16 +1558,16 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>2.15e-18</v>
+        <v>1.348</v>
       </c>
       <c r="D57" t="n">
-        <v>6.439</v>
+        <v>5.283</v>
       </c>
       <c r="E57" t="n">
-        <v>1.968</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58">
@@ -1578,16 +1578,16 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>3.592e-18</v>
+        <v>1.832</v>
       </c>
       <c r="D58" t="n">
-        <v>4.914</v>
+        <v>5.019</v>
       </c>
       <c r="E58" t="n">
-        <v>1.268</v>
+        <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59">
@@ -1598,16 +1598,16 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>1.538e-18</v>
+        <v>0.3051</v>
       </c>
       <c r="D59" t="n">
-        <v>5.414</v>
+        <v>5.137</v>
       </c>
       <c r="E59" t="n">
-        <v>0.3571</v>
+        <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60">
@@ -1618,16 +1618,16 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>8.575e-19</v>
+        <v>1.797</v>
       </c>
       <c r="D60" t="n">
-        <v>6.023</v>
+        <v>4.918</v>
       </c>
       <c r="E60" t="n">
-        <v>0.2395</v>
+        <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61">
@@ -1641,13 +1641,13 @@
         <v>0.194</v>
       </c>
       <c r="D61" t="n">
-        <v>6.576</v>
+        <v>4.895</v>
       </c>
       <c r="E61" t="n">
-        <v>0.1818</v>
+        <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62">
@@ -1661,13 +1661,13 @@
         <v>0.147</v>
       </c>
       <c r="D62" t="n">
-        <v>6.771</v>
+        <v>4.801</v>
       </c>
       <c r="E62" t="n">
-        <v>0.1987</v>
+        <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63">
@@ -1678,16 +1678,16 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>1.016e-17</v>
+        <v>0.216</v>
       </c>
       <c r="D63" t="n">
-        <v>6.383</v>
+        <v>4.72</v>
       </c>
       <c r="E63" t="n">
-        <v>0.9268999999999999</v>
+        <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64">
@@ -1698,16 +1698,16 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>8.577e-19</v>
+        <v>0.1372</v>
       </c>
       <c r="D64" t="n">
-        <v>5.523</v>
+        <v>4.639</v>
       </c>
       <c r="E64" t="n">
-        <v>1.142</v>
+        <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65">
@@ -1718,13 +1718,13 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>6.728e-18</v>
+        <v>0.004142</v>
       </c>
       <c r="D65" t="n">
-        <v>6.621</v>
+        <v>5.546</v>
       </c>
       <c r="E65" t="n">
-        <v>1.437</v>
+        <v>0.2186</v>
       </c>
       <c r="F65" t="n">
         <v>5</v>
@@ -1738,16 +1738,16 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>1.294e-17</v>
+        <v>0.01208</v>
       </c>
       <c r="D66" t="n">
-        <v>7.142</v>
+        <v>4.676</v>
       </c>
       <c r="E66" t="n">
-        <v>2.165</v>
+        <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
@@ -1758,16 +1758,16 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>7.243e-19</v>
+        <v>0.01316</v>
       </c>
       <c r="D67" t="n">
-        <v>6.465</v>
+        <v>4.738</v>
       </c>
       <c r="E67" t="n">
-        <v>1.611</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68">
@@ -1778,16 +1778,16 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>2.539e-19</v>
+        <v>0.1508</v>
       </c>
       <c r="D68" t="n">
-        <v>7.099</v>
+        <v>4.885</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5243</v>
+        <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69">
@@ -1798,16 +1798,16 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>0.006925</v>
+        <v>0.1178</v>
       </c>
       <c r="D69" t="n">
-        <v>4.937</v>
+        <v>5.017</v>
       </c>
       <c r="E69" t="n">
-        <v>0.2123</v>
+        <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70">
@@ -1818,13 +1818,13 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.0007808</v>
+        <v>0.02316</v>
       </c>
       <c r="D70" t="n">
-        <v>4.815</v>
+        <v>5.41</v>
       </c>
       <c r="E70" t="n">
-        <v>0.3495</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
         <v>10</v>
@@ -1838,16 +1838,16 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>1.359e-19</v>
+        <v>0.3763</v>
       </c>
       <c r="D71" t="n">
-        <v>6.906</v>
+        <v>5.059</v>
       </c>
       <c r="E71" t="n">
-        <v>1.134</v>
+        <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72">
@@ -1858,16 +1858,16 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>7.207e-19</v>
+        <v>0.02234</v>
       </c>
       <c r="D72" t="n">
-        <v>8.228</v>
+        <v>5.85</v>
       </c>
       <c r="E72" t="n">
-        <v>0.9114</v>
+        <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 05-06-2024 at 22:09
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -458,16 +458,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>2.473e-19</v>
+        <v>0.08511000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>1.602</v>
+        <v>0.5594</v>
       </c>
       <c r="E2" t="n">
-        <v>0.526</v>
+        <v>29.39</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1.81e-18</v>
+        <v>0.6979</v>
       </c>
       <c r="D3" t="n">
-        <v>2.529</v>
+        <v>0.6743</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5928</v>
+        <v>5.193</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -498,16 +498,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3462</v>
+        <v>0.6943</v>
       </c>
       <c r="D4" t="n">
-        <v>1.323</v>
+        <v>0.6717</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2749</v>
+        <v>2.554</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -518,16 +518,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3308</v>
+        <v>0.4422</v>
       </c>
       <c r="D5" t="n">
-        <v>0.74</v>
+        <v>1.353</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1534</v>
+        <v>6.515</v>
       </c>
       <c r="F5" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1351</v>
+        <v>0.3291</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8452</v>
+        <v>1.443</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1706</v>
+        <v>4.434</v>
       </c>
       <c r="F6" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -558,16 +558,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06888</v>
+        <v>0.3268</v>
       </c>
       <c r="D7" t="n">
-        <v>1.4</v>
+        <v>1.498</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4627</v>
+        <v>1.808</v>
       </c>
       <c r="F7" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -578,16 +578,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.05829</v>
+        <v>0.08572</v>
       </c>
       <c r="D8" t="n">
-        <v>1.679</v>
+        <v>1.398</v>
       </c>
       <c r="E8" t="n">
-        <v>1.399</v>
+        <v>12.8</v>
       </c>
       <c r="F8" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2477</v>
+        <v>0.2293</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1.712</v>
       </c>
       <c r="E9" t="n">
-        <v>1.228</v>
+        <v>8.132</v>
       </c>
       <c r="F9" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -621,13 +621,13 @@
         <v>0.4646</v>
       </c>
       <c r="D10" t="n">
-        <v>1.501</v>
+        <v>1.681</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5923</v>
+        <v>8.157</v>
       </c>
       <c r="F10" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -638,16 +638,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4228</v>
+        <v>0.5077</v>
       </c>
       <c r="D11" t="n">
-        <v>1.605</v>
+        <v>1.704</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1071</v>
+        <v>1.981</v>
       </c>
       <c r="F11" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -658,16 +658,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3204</v>
+        <v>0.3098</v>
       </c>
       <c r="D12" t="n">
-        <v>1.748</v>
+        <v>1.638</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7953</v>
+        <v>0.2045</v>
       </c>
       <c r="F12" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
@@ -678,16 +678,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.002187</v>
+        <v>0.3686</v>
       </c>
       <c r="D13" t="n">
-        <v>1.837</v>
+        <v>1.656</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1693</v>
+        <v>3.84</v>
       </c>
       <c r="F13" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
@@ -698,16 +698,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1009</v>
+        <v>0.01326</v>
       </c>
       <c r="D14" t="n">
-        <v>2.557</v>
+        <v>2.343</v>
       </c>
       <c r="E14" t="n">
-        <v>0.3006</v>
+        <v>1.956</v>
       </c>
       <c r="F14" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -718,16 +718,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.1076</v>
       </c>
       <c r="D15" t="n">
-        <v>2.735</v>
+        <v>2.419</v>
       </c>
       <c r="E15" t="n">
-        <v>0.242</v>
+        <v>1.707</v>
       </c>
       <c r="F15" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -738,16 +738,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.00134</v>
+        <v>0.01744</v>
       </c>
       <c r="D16" t="n">
-        <v>2.518</v>
+        <v>2.7</v>
       </c>
       <c r="E16" t="n">
-        <v>0.7192</v>
+        <v>0.7079</v>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -758,16 +758,16 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0002662</v>
+        <v>0.001435</v>
       </c>
       <c r="D17" t="n">
-        <v>2.7</v>
+        <v>3.088</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2886</v>
+        <v>1.282</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -778,16 +778,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.007861</v>
+        <v>0.02765</v>
       </c>
       <c r="D18" t="n">
-        <v>3.241</v>
+        <v>2.91</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2737</v>
+        <v>1.842</v>
       </c>
       <c r="F18" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -798,16 +798,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1738</v>
+        <v>0.2279</v>
       </c>
       <c r="D19" t="n">
-        <v>2.823</v>
+        <v>2.772</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2202</v>
+        <v>1.935</v>
       </c>
       <c r="F19" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -818,16 +818,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01123</v>
+        <v>0.03506</v>
       </c>
       <c r="D20" t="n">
-        <v>3.415</v>
+        <v>3.269</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2173</v>
+        <v>7.147</v>
       </c>
       <c r="F20" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -838,16 +838,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0126</v>
+        <v>0.03532</v>
       </c>
       <c r="D21" t="n">
-        <v>3.535</v>
+        <v>3.488</v>
       </c>
       <c r="E21" t="n">
-        <v>0.107</v>
+        <v>0.7301</v>
       </c>
       <c r="F21" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
@@ -858,16 +858,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.008581999999999999</v>
+        <v>0.005181</v>
       </c>
       <c r="D22" t="n">
-        <v>3.501</v>
+        <v>3.814</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1225</v>
+        <v>4.715</v>
       </c>
       <c r="F22" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -878,13 +878,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.03624</v>
+        <v>0.262</v>
       </c>
       <c r="D23" t="n">
-        <v>3.327</v>
+        <v>2.95</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4257</v>
+        <v>1.506</v>
       </c>
       <c r="F23" t="n">
         <v>25</v>
@@ -898,13 +898,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01635</v>
+        <v>0.1853</v>
       </c>
       <c r="D24" t="n">
-        <v>3.508</v>
+        <v>3.051</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6127</v>
+        <v>1.543</v>
       </c>
       <c r="F24" t="n">
         <v>25</v>
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.009377</v>
+        <v>0.001472</v>
       </c>
       <c r="D25" t="n">
-        <v>4.187</v>
+        <v>4.944</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6296</v>
+        <v>3.34</v>
       </c>
       <c r="F25" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -938,16 +938,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01314</v>
+        <v>0.01113</v>
       </c>
       <c r="D26" t="n">
-        <v>4.131</v>
+        <v>4.415</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1966</v>
+        <v>0.1375</v>
       </c>
       <c r="F26" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -958,16 +958,16 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01183</v>
+        <v>0.006732</v>
       </c>
       <c r="D27" t="n">
-        <v>4.956</v>
+        <v>4.759</v>
       </c>
       <c r="E27" t="n">
-        <v>0.3537</v>
+        <v>2.331</v>
       </c>
       <c r="F27" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -978,16 +978,16 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0006742</v>
+        <v>0.02502</v>
       </c>
       <c r="D28" t="n">
-        <v>4.715</v>
+        <v>4.724</v>
       </c>
       <c r="E28" t="n">
-        <v>0.526</v>
+        <v>0.4165</v>
       </c>
       <c r="F28" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
@@ -998,16 +998,16 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02656</v>
+        <v>0.01393</v>
       </c>
       <c r="D29" t="n">
-        <v>4.982</v>
+        <v>4.784</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1488</v>
+        <v>2.841</v>
       </c>
       <c r="F29" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -1018,16 +1018,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0008779</v>
+        <v>0.001821</v>
       </c>
       <c r="D30" t="n">
-        <v>5.018</v>
+        <v>5.247</v>
       </c>
       <c r="E30" t="n">
-        <v>0.2842</v>
+        <v>1.1</v>
       </c>
       <c r="F30" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -1038,16 +1038,16 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.06807000000000001</v>
+        <v>0.1107</v>
       </c>
       <c r="D31" t="n">
-        <v>4.629</v>
+        <v>4.248</v>
       </c>
       <c r="E31" t="n">
-        <v>0.253</v>
+        <v>1.844</v>
       </c>
       <c r="F31" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
@@ -1058,16 +1058,16 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0004758</v>
+        <v>0.143</v>
       </c>
       <c r="D32" t="n">
-        <v>4.611</v>
+        <v>4.078</v>
       </c>
       <c r="E32" t="n">
-        <v>0.6179</v>
+        <v>1.283</v>
       </c>
       <c r="F32" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33">
@@ -1078,16 +1078,16 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01389</v>
+        <v>0.1074</v>
       </c>
       <c r="D33" t="n">
-        <v>5.115</v>
+        <v>4.168</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2695</v>
+        <v>0.5926</v>
       </c>
       <c r="F33" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34">
@@ -1098,16 +1098,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.005308</v>
+        <v>0.001119</v>
       </c>
       <c r="D34" t="n">
-        <v>5.212</v>
+        <v>4.909</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3045</v>
+        <v>3.076</v>
       </c>
       <c r="F34" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
@@ -1118,16 +1118,16 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.001326</v>
+        <v>0.005295</v>
       </c>
       <c r="D35" t="n">
-        <v>5.081</v>
+        <v>4.934</v>
       </c>
       <c r="E35" t="n">
-        <v>0.164</v>
+        <v>1.274</v>
       </c>
       <c r="F35" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
@@ -1138,16 +1138,16 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0005083</v>
+        <v>0.0006306</v>
       </c>
       <c r="D36" t="n">
-        <v>5.216</v>
+        <v>5.988</v>
       </c>
       <c r="E36" t="n">
-        <v>0.2042</v>
+        <v>0.1078</v>
       </c>
       <c r="F36" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -1161,13 +1161,13 @@
         <v>0.07881000000000001</v>
       </c>
       <c r="D37" t="n">
-        <v>4.952</v>
+        <v>5.077</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2847</v>
+        <v>3.407</v>
       </c>
       <c r="F37" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
@@ -1178,16 +1178,16 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.06856</v>
+        <v>0.1844</v>
       </c>
       <c r="D38" t="n">
-        <v>4.969</v>
+        <v>4.817</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4637</v>
+        <v>2.233</v>
       </c>
       <c r="F38" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39">
@@ -1198,16 +1198,16 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.03904</v>
+        <v>0.2017</v>
       </c>
       <c r="D39" t="n">
-        <v>5.004</v>
+        <v>4.739</v>
       </c>
       <c r="E39" t="n">
-        <v>0.7395</v>
+        <v>0.552</v>
       </c>
       <c r="F39" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40">
@@ -1218,16 +1218,16 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01848</v>
+        <v>0.1572</v>
       </c>
       <c r="D40" t="n">
-        <v>5.541</v>
+        <v>4.71</v>
       </c>
       <c r="E40" t="n">
-        <v>0.2089</v>
+        <v>0.7847</v>
       </c>
       <c r="F40" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41">
@@ -1238,16 +1238,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.006495</v>
+        <v>0.01794</v>
       </c>
       <c r="D41" t="n">
-        <v>5.604</v>
+        <v>5.191</v>
       </c>
       <c r="E41" t="n">
-        <v>0.08316999999999999</v>
+        <v>2.433</v>
       </c>
       <c r="F41" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42">
@@ -1258,16 +1258,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.003861</v>
+        <v>0.01892</v>
       </c>
       <c r="D42" t="n">
-        <v>5.56</v>
+        <v>5.273</v>
       </c>
       <c r="E42" t="n">
-        <v>0.3786</v>
+        <v>0.6876</v>
       </c>
       <c r="F42" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43">
@@ -1278,16 +1278,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1434</v>
+        <v>0.1761</v>
       </c>
       <c r="D43" t="n">
-        <v>5.145</v>
+        <v>5.155</v>
       </c>
       <c r="E43" t="n">
-        <v>0.2819</v>
+        <v>5.025</v>
       </c>
       <c r="F43" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44">
@@ -1298,16 +1298,16 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.229</v>
+        <v>0.1483</v>
       </c>
       <c r="D44" t="n">
-        <v>5.203</v>
+        <v>4.914</v>
       </c>
       <c r="E44" t="n">
-        <v>1.989</v>
+        <v>6.448</v>
       </c>
       <c r="F44" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45">
@@ -1318,16 +1318,16 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.01825</v>
+        <v>0.1142</v>
       </c>
       <c r="D45" t="n">
-        <v>5.361</v>
+        <v>4.866</v>
       </c>
       <c r="E45" t="n">
-        <v>2.31</v>
+        <v>4.086</v>
       </c>
       <c r="F45" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46">
@@ -1338,16 +1338,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1221</v>
+        <v>0.1509</v>
       </c>
       <c r="D46" t="n">
-        <v>5.839</v>
+        <v>5.466</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4614</v>
+        <v>5.745</v>
       </c>
       <c r="F46" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47">
@@ -1358,16 +1358,16 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2315</v>
+        <v>0.1562</v>
       </c>
       <c r="D47" t="n">
-        <v>5.903</v>
+        <v>4.916</v>
       </c>
       <c r="E47" t="n">
-        <v>0.6021</v>
+        <v>5.119</v>
       </c>
       <c r="F47" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48">
@@ -1378,16 +1378,16 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>0.406</v>
+        <v>0.07398</v>
       </c>
       <c r="D48" t="n">
-        <v>5.547</v>
+        <v>5.848</v>
       </c>
       <c r="E48" t="n">
-        <v>0.144</v>
+        <v>4.137</v>
       </c>
       <c r="F48" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>1.754e-18</v>
+        <v>0.2396</v>
       </c>
       <c r="D49" t="n">
-        <v>7.939</v>
+        <v>5.176</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5756</v>
+        <v>2.015</v>
       </c>
       <c r="F49" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50">
@@ -1418,16 +1418,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.03743</v>
+        <v>0.1907</v>
       </c>
       <c r="D50" t="n">
-        <v>6.44</v>
+        <v>4.994</v>
       </c>
       <c r="E50" t="n">
-        <v>1.615</v>
+        <v>1.27</v>
       </c>
       <c r="F50" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
@@ -1438,16 +1438,16 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>1.261e-17</v>
+        <v>0.002616</v>
       </c>
       <c r="D51" t="n">
-        <v>7.616</v>
+        <v>6.348</v>
       </c>
       <c r="E51" t="n">
-        <v>0.9634</v>
+        <v>5.16</v>
       </c>
       <c r="F51" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1458,16 +1458,16 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>0.02474</v>
+        <v>0.0207</v>
       </c>
       <c r="D52" t="n">
-        <v>6.173</v>
+        <v>5.95</v>
       </c>
       <c r="E52" t="n">
-        <v>1.329</v>
+        <v>4.706</v>
       </c>
       <c r="F52" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53">
@@ -1481,13 +1481,13 @@
         <v>0.08151</v>
       </c>
       <c r="D53" t="n">
-        <v>5.96</v>
+        <v>5.723</v>
       </c>
       <c r="E53" t="n">
-        <v>0.3352</v>
+        <v>3.793</v>
       </c>
       <c r="F53" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54">
@@ -1498,16 +1498,16 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.6843</v>
+        <v>0.8924</v>
       </c>
       <c r="D54" t="n">
-        <v>5.491</v>
+        <v>5.521</v>
       </c>
       <c r="E54" t="n">
-        <v>0.4235</v>
+        <v>2.419</v>
       </c>
       <c r="F54" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55">
@@ -1518,16 +1518,16 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.3566</v>
+        <v>0.04006</v>
       </c>
       <c r="D55" t="n">
-        <v>5.392</v>
+        <v>5.256</v>
       </c>
       <c r="E55" t="n">
-        <v>1.096</v>
+        <v>7.908</v>
       </c>
       <c r="F55" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56">
@@ -1538,16 +1538,16 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.07369000000000001</v>
+        <v>0.06797</v>
       </c>
       <c r="D56" t="n">
-        <v>5.366</v>
+        <v>5.319</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1319</v>
+        <v>5.223</v>
       </c>
       <c r="F56" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57">
@@ -1558,16 +1558,16 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.02181</v>
+        <v>0.008366999999999999</v>
       </c>
       <c r="D57" t="n">
-        <v>5.205</v>
+        <v>5.015</v>
       </c>
       <c r="E57" t="n">
-        <v>0.6167</v>
+        <v>8.787000000000001</v>
       </c>
       <c r="F57" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58">
@@ -1578,16 +1578,16 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>0.01284</v>
+        <v>0.01629</v>
       </c>
       <c r="D58" t="n">
-        <v>4.392</v>
+        <v>4.782</v>
       </c>
       <c r="E58" t="n">
-        <v>0.361</v>
+        <v>11.29</v>
       </c>
       <c r="F58" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
@@ -1598,16 +1598,16 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.243</v>
+        <v>0.3051</v>
       </c>
       <c r="D59" t="n">
-        <v>4.955</v>
+        <v>5.119</v>
       </c>
       <c r="E59" t="n">
-        <v>0.3571</v>
+        <v>2.438</v>
       </c>
       <c r="F59" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60">
@@ -1618,16 +1618,16 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>0.02578</v>
+        <v>0.03417</v>
       </c>
       <c r="D60" t="n">
-        <v>4.763</v>
+        <v>4.528</v>
       </c>
       <c r="E60" t="n">
-        <v>0.07553</v>
+        <v>5.903</v>
       </c>
       <c r="F60" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61">
@@ -1638,16 +1638,16 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>0.194</v>
+        <v>0.05077</v>
       </c>
       <c r="D61" t="n">
-        <v>4.809</v>
+        <v>4.683</v>
       </c>
       <c r="E61" t="n">
-        <v>0.1818</v>
+        <v>0.2774</v>
       </c>
       <c r="F61" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62">
@@ -1661,13 +1661,13 @@
         <v>0.147</v>
       </c>
       <c r="D62" t="n">
-        <v>4.719</v>
+        <v>4.784</v>
       </c>
       <c r="E62" t="n">
-        <v>0.1987</v>
+        <v>1.055</v>
       </c>
       <c r="F62" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63">
@@ -1678,16 +1678,16 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1728</v>
+        <v>0.216</v>
       </c>
       <c r="D63" t="n">
-        <v>4.714</v>
+        <v>4.747</v>
       </c>
       <c r="E63" t="n">
-        <v>0.9268999999999999</v>
+        <v>2.31</v>
       </c>
       <c r="F63" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64">
@@ -1698,16 +1698,16 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>0.006758</v>
+        <v>0.009783</v>
       </c>
       <c r="D64" t="n">
-        <v>4.34</v>
+        <v>4.563</v>
       </c>
       <c r="E64" t="n">
-        <v>0.5497</v>
+        <v>6.836</v>
       </c>
       <c r="F64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65">
@@ -1718,16 +1718,16 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.009176</v>
+        <v>0.005106</v>
       </c>
       <c r="D65" t="n">
-        <v>4.839</v>
+        <v>5.132</v>
       </c>
       <c r="E65" t="n">
-        <v>0.2289</v>
+        <v>6.556</v>
       </c>
       <c r="F65" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -1738,16 +1738,16 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.002954</v>
+        <v>0.02205</v>
       </c>
       <c r="D66" t="n">
-        <v>4.865</v>
+        <v>4.764</v>
       </c>
       <c r="E66" t="n">
-        <v>1.317</v>
+        <v>5.25</v>
       </c>
       <c r="F66" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67">
@@ -1758,16 +1758,16 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>9.974e-05</v>
+        <v>0.01528</v>
       </c>
       <c r="D67" t="n">
-        <v>5.142</v>
+        <v>4.891</v>
       </c>
       <c r="E67" t="n">
-        <v>0.3696</v>
+        <v>3.808</v>
       </c>
       <c r="F67" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68">
@@ -1778,16 +1778,16 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1508</v>
+        <v>0.1135</v>
       </c>
       <c r="D68" t="n">
-        <v>4.836</v>
+        <v>4.952</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5243</v>
+        <v>3.493</v>
       </c>
       <c r="F68" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69">
@@ -1798,16 +1798,16 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>0.006925</v>
+        <v>0.1673</v>
       </c>
       <c r="D69" t="n">
-        <v>5.666</v>
+        <v>4.934</v>
       </c>
       <c r="E69" t="n">
-        <v>0.1013</v>
+        <v>1.581</v>
       </c>
       <c r="F69" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70">
@@ -1818,16 +1818,16 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.02144</v>
+        <v>0.02316</v>
       </c>
       <c r="D70" t="n">
-        <v>6.043</v>
+        <v>5.525</v>
       </c>
       <c r="E70" t="n">
-        <v>0.0873</v>
+        <v>2.211</v>
       </c>
       <c r="F70" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71">
@@ -1838,16 +1838,16 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.006183</v>
+        <v>0.3763</v>
       </c>
       <c r="D71" t="n">
-        <v>5.847</v>
+        <v>4.82</v>
       </c>
       <c r="E71" t="n">
-        <v>0.5238</v>
+        <v>0.2145</v>
       </c>
       <c r="F71" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72">
@@ -1861,13 +1861,13 @@
         <v>0.02639</v>
       </c>
       <c r="D72" t="n">
-        <v>6.084</v>
+        <v>5.799</v>
       </c>
       <c r="E72" t="n">
-        <v>0.3582</v>
+        <v>0.475</v>
       </c>
       <c r="F72" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 05-13-2024 at 18:11
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -458,16 +458,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08511000000000001</v>
+        <v>7.16e-19</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5594</v>
+        <v>1.352</v>
       </c>
       <c r="E2" t="n">
-        <v>29.39</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6979</v>
+        <v>0.39</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6743</v>
+        <v>1.087</v>
       </c>
       <c r="E3" t="n">
-        <v>5.193</v>
+        <v>8.346</v>
       </c>
       <c r="F3" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -498,16 +498,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6943</v>
+        <v>0.403</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6717</v>
+        <v>1.087</v>
       </c>
       <c r="E4" t="n">
-        <v>2.554</v>
+        <v>3.376</v>
       </c>
       <c r="F4" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -518,16 +518,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4422</v>
+        <v>0.4956</v>
       </c>
       <c r="D5" t="n">
-        <v>1.353</v>
+        <v>1.283</v>
       </c>
       <c r="E5" t="n">
-        <v>6.515</v>
+        <v>0.4391</v>
       </c>
       <c r="F5" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3291</v>
+        <v>0.3475</v>
       </c>
       <c r="D6" t="n">
-        <v>1.443</v>
+        <v>1.216</v>
       </c>
       <c r="E6" t="n">
-        <v>4.434</v>
+        <v>1.154</v>
       </c>
       <c r="F6" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -558,16 +558,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3268</v>
+        <v>0.01168</v>
       </c>
       <c r="D7" t="n">
-        <v>1.498</v>
+        <v>1.925</v>
       </c>
       <c r="E7" t="n">
-        <v>1.808</v>
+        <v>2.734</v>
       </c>
       <c r="F7" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -578,16 +578,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08572</v>
+        <v>0.7325</v>
       </c>
       <c r="D8" t="n">
-        <v>1.398</v>
+        <v>1.411</v>
       </c>
       <c r="E8" t="n">
-        <v>12.8</v>
+        <v>4.85</v>
       </c>
       <c r="F8" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2293</v>
+        <v>0.07799</v>
       </c>
       <c r="D9" t="n">
-        <v>1.712</v>
+        <v>2.249</v>
       </c>
       <c r="E9" t="n">
         <v>8.132</v>
       </c>
       <c r="F9" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -618,16 +618,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4646</v>
+        <v>0.165</v>
       </c>
       <c r="D10" t="n">
-        <v>1.681</v>
+        <v>1.887</v>
       </c>
       <c r="E10" t="n">
         <v>8.157</v>
       </c>
       <c r="F10" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -638,16 +638,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5077</v>
+        <v>0.158</v>
       </c>
       <c r="D11" t="n">
-        <v>1.704</v>
+        <v>1.893</v>
       </c>
       <c r="E11" t="n">
         <v>1.981</v>
       </c>
       <c r="F11" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -658,16 +658,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3098</v>
+        <v>0.2192</v>
       </c>
       <c r="D12" t="n">
-        <v>1.638</v>
+        <v>1.961</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2045</v>
+        <v>5.746</v>
       </c>
       <c r="F12" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -678,16 +678,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3686</v>
+        <v>0.244</v>
       </c>
       <c r="D13" t="n">
-        <v>1.656</v>
+        <v>2.067</v>
       </c>
       <c r="E13" t="n">
-        <v>3.84</v>
+        <v>0.1693</v>
       </c>
       <c r="F13" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -698,16 +698,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01326</v>
+        <v>0.2771</v>
       </c>
       <c r="D14" t="n">
-        <v>2.343</v>
+        <v>2.147</v>
       </c>
       <c r="E14" t="n">
-        <v>1.956</v>
+        <v>1.517</v>
       </c>
       <c r="F14" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
@@ -718,16 +718,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1076</v>
+        <v>0.8951</v>
       </c>
       <c r="D15" t="n">
-        <v>2.419</v>
+        <v>1.877</v>
       </c>
       <c r="E15" t="n">
-        <v>1.707</v>
+        <v>2.119</v>
       </c>
       <c r="F15" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -738,16 +738,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01744</v>
+        <v>0.00134</v>
       </c>
       <c r="D16" t="n">
-        <v>2.7</v>
+        <v>2.986</v>
       </c>
       <c r="E16" t="n">
         <v>0.7079</v>
       </c>
       <c r="F16" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -758,16 +758,16 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.001435</v>
+        <v>8.933000000000001e-19</v>
       </c>
       <c r="D17" t="n">
-        <v>3.088</v>
+        <v>4.673</v>
       </c>
       <c r="E17" t="n">
-        <v>1.282</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -778,16 +778,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.02765</v>
+        <v>0.003378</v>
       </c>
       <c r="D18" t="n">
-        <v>2.91</v>
+        <v>3.301</v>
       </c>
       <c r="E18" t="n">
         <v>1.842</v>
       </c>
       <c r="F18" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -798,16 +798,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2279</v>
+        <v>0.0537</v>
       </c>
       <c r="D19" t="n">
-        <v>2.772</v>
+        <v>2.855</v>
       </c>
       <c r="E19" t="n">
-        <v>1.935</v>
+        <v>1.833</v>
       </c>
       <c r="F19" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -818,16 +818,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.03506</v>
+        <v>0.03501</v>
       </c>
       <c r="D20" t="n">
-        <v>3.269</v>
+        <v>3.166</v>
       </c>
       <c r="E20" t="n">
-        <v>7.147</v>
+        <v>3.975</v>
       </c>
       <c r="F20" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -838,16 +838,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.03532</v>
+        <v>0.03476</v>
       </c>
       <c r="D21" t="n">
-        <v>3.488</v>
+        <v>3.315</v>
       </c>
       <c r="E21" t="n">
-        <v>0.7301</v>
+        <v>2.251</v>
       </c>
       <c r="F21" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
@@ -858,16 +858,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.005181</v>
+        <v>0.03365</v>
       </c>
       <c r="D22" t="n">
-        <v>3.814</v>
+        <v>3.471</v>
       </c>
       <c r="E22" t="n">
-        <v>4.715</v>
+        <v>2.27</v>
       </c>
       <c r="F22" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -878,16 +878,16 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.262</v>
+        <v>0.07542</v>
       </c>
       <c r="D23" t="n">
-        <v>2.95</v>
+        <v>3.46</v>
       </c>
       <c r="E23" t="n">
-        <v>1.506</v>
+        <v>2.956</v>
       </c>
       <c r="F23" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24">
@@ -898,16 +898,16 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1853</v>
+        <v>0.1338</v>
       </c>
       <c r="D24" t="n">
-        <v>3.051</v>
+        <v>3.465</v>
       </c>
       <c r="E24" t="n">
-        <v>1.543</v>
+        <v>1.083</v>
       </c>
       <c r="F24" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.001472</v>
+        <v>0.1851</v>
       </c>
       <c r="D25" t="n">
-        <v>4.944</v>
+        <v>3.375</v>
       </c>
       <c r="E25" t="n">
-        <v>3.34</v>
+        <v>0.6208</v>
       </c>
       <c r="F25" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
@@ -938,16 +938,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01113</v>
+        <v>0.429</v>
       </c>
       <c r="D26" t="n">
-        <v>4.415</v>
+        <v>7.131</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1375</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -958,16 +958,16 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.006732</v>
+        <v>1.262e-29</v>
       </c>
       <c r="D27" t="n">
-        <v>4.759</v>
+        <v>6.608</v>
       </c>
       <c r="E27" t="n">
-        <v>2.331</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
@@ -978,16 +978,16 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02502</v>
+        <v>0.001944</v>
       </c>
       <c r="D28" t="n">
-        <v>4.724</v>
+        <v>5.613</v>
       </c>
       <c r="E28" t="n">
-        <v>0.4165</v>
+        <v>1.064</v>
       </c>
       <c r="F28" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -998,16 +998,16 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.01393</v>
+        <v>0.002924</v>
       </c>
       <c r="D29" t="n">
-        <v>4.784</v>
+        <v>5.429</v>
       </c>
       <c r="E29" t="n">
         <v>2.841</v>
       </c>
       <c r="F29" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
@@ -1018,16 +1018,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.001821</v>
+        <v>0.2944</v>
       </c>
       <c r="D30" t="n">
-        <v>5.247</v>
+        <v>8.938000000000001</v>
       </c>
       <c r="E30" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1038,16 +1038,16 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1107</v>
+        <v>0.01533</v>
       </c>
       <c r="D31" t="n">
-        <v>4.248</v>
+        <v>5.019</v>
       </c>
       <c r="E31" t="n">
-        <v>1.844</v>
+        <v>0.9826</v>
       </c>
       <c r="F31" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
@@ -1058,16 +1058,16 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.143</v>
+        <v>0.1035</v>
       </c>
       <c r="D32" t="n">
-        <v>4.078</v>
+        <v>4.556</v>
       </c>
       <c r="E32" t="n">
-        <v>1.283</v>
+        <v>0.764</v>
       </c>
       <c r="F32" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
@@ -1078,16 +1078,16 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1074</v>
+        <v>0.0824</v>
       </c>
       <c r="D33" t="n">
-        <v>4.168</v>
+        <v>4.61</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5926</v>
+        <v>1.01</v>
       </c>
       <c r="F33" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34">
@@ -1098,16 +1098,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.001119</v>
+        <v>0.1264</v>
       </c>
       <c r="D34" t="n">
-        <v>4.909</v>
+        <v>4.457</v>
       </c>
       <c r="E34" t="n">
-        <v>3.076</v>
+        <v>0.301</v>
       </c>
       <c r="F34" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
@@ -1118,16 +1118,16 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.005295</v>
+        <v>0.104</v>
       </c>
       <c r="D35" t="n">
-        <v>4.934</v>
+        <v>4.554</v>
       </c>
       <c r="E35" t="n">
-        <v>1.274</v>
+        <v>0.6122</v>
       </c>
       <c r="F35" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36">
@@ -1138,16 +1138,16 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0006306</v>
+        <v>2.312e-19</v>
       </c>
       <c r="D36" t="n">
-        <v>5.988</v>
+        <v>7.081</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1078</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1158,16 +1158,16 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.07881000000000001</v>
+        <v>0.01241</v>
       </c>
       <c r="D37" t="n">
-        <v>5.077</v>
+        <v>5.121</v>
       </c>
       <c r="E37" t="n">
         <v>3.407</v>
       </c>
       <c r="F37" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
@@ -1178,16 +1178,16 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1844</v>
+        <v>0.04219</v>
       </c>
       <c r="D38" t="n">
-        <v>4.817</v>
+        <v>5.038</v>
       </c>
       <c r="E38" t="n">
-        <v>2.233</v>
+        <v>0.8683999999999999</v>
       </c>
       <c r="F38" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
@@ -1198,16 +1198,16 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.2017</v>
+        <v>0.03904</v>
       </c>
       <c r="D39" t="n">
-        <v>4.739</v>
+        <v>5.085</v>
       </c>
       <c r="E39" t="n">
         <v>0.552</v>
       </c>
       <c r="F39" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40">
@@ -1218,16 +1218,16 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1572</v>
+        <v>0.06263000000000001</v>
       </c>
       <c r="D40" t="n">
-        <v>4.71</v>
+        <v>5.082</v>
       </c>
       <c r="E40" t="n">
-        <v>0.7847</v>
+        <v>1.165</v>
       </c>
       <c r="F40" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41">
@@ -1238,16 +1238,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.01794</v>
+        <v>0.1733</v>
       </c>
       <c r="D41" t="n">
-        <v>5.191</v>
+        <v>4.953</v>
       </c>
       <c r="E41" t="n">
-        <v>2.433</v>
+        <v>0.07194</v>
       </c>
       <c r="F41" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42">
@@ -1258,16 +1258,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01892</v>
+        <v>0.00175</v>
       </c>
       <c r="D42" t="n">
-        <v>5.273</v>
+        <v>5.667</v>
       </c>
       <c r="E42" t="n">
         <v>0.6876</v>
       </c>
       <c r="F42" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -1278,16 +1278,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1761</v>
+        <v>0.02719</v>
       </c>
       <c r="D43" t="n">
-        <v>5.155</v>
+        <v>5.177</v>
       </c>
       <c r="E43" t="n">
         <v>5.025</v>
       </c>
       <c r="F43" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
@@ -1298,16 +1298,16 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1483</v>
+        <v>0.6196</v>
       </c>
       <c r="D44" t="n">
-        <v>4.914</v>
+        <v>5.13</v>
       </c>
       <c r="E44" t="n">
-        <v>6.448</v>
+        <v>5.344</v>
       </c>
       <c r="F44" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45">
@@ -1318,16 +1318,16 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1142</v>
+        <v>0.5965</v>
       </c>
       <c r="D45" t="n">
-        <v>4.866</v>
+        <v>5.141</v>
       </c>
       <c r="E45" t="n">
-        <v>4.086</v>
+        <v>2.722</v>
       </c>
       <c r="F45" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46">
@@ -1338,16 +1338,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1509</v>
+        <v>0.00479</v>
       </c>
       <c r="D46" t="n">
-        <v>5.466</v>
+        <v>6.554</v>
       </c>
       <c r="E46" t="n">
         <v>5.745</v>
       </c>
       <c r="F46" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -1358,16 +1358,16 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1562</v>
+        <v>0.06633</v>
       </c>
       <c r="D47" t="n">
-        <v>4.916</v>
+        <v>5.719</v>
       </c>
       <c r="E47" t="n">
-        <v>5.119</v>
+        <v>1.158</v>
       </c>
       <c r="F47" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
@@ -1378,16 +1378,16 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>0.07398</v>
+        <v>1.252e-19</v>
       </c>
       <c r="D48" t="n">
-        <v>5.848</v>
+        <v>7.863</v>
       </c>
       <c r="E48" t="n">
-        <v>4.137</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2396</v>
+        <v>0.1792</v>
       </c>
       <c r="D49" t="n">
-        <v>5.176</v>
+        <v>5.803</v>
       </c>
       <c r="E49" t="n">
-        <v>2.015</v>
+        <v>0.9627</v>
       </c>
       <c r="F49" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50">
@@ -1418,16 +1418,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1907</v>
+        <v>1.037</v>
       </c>
       <c r="D50" t="n">
-        <v>4.994</v>
+        <v>5.371</v>
       </c>
       <c r="E50" t="n">
         <v>1.27</v>
       </c>
       <c r="F50" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51">
@@ -1438,16 +1438,16 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>0.002616</v>
+        <v>1.367</v>
       </c>
       <c r="D51" t="n">
-        <v>6.348</v>
+        <v>9.071</v>
       </c>
       <c r="E51" t="n">
-        <v>5.16</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -1458,16 +1458,16 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0207</v>
+        <v>1.349e-18</v>
       </c>
       <c r="D52" t="n">
-        <v>5.95</v>
+        <v>7.858</v>
       </c>
       <c r="E52" t="n">
-        <v>4.706</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -1478,16 +1478,16 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>0.08151</v>
+        <v>0.03151</v>
       </c>
       <c r="D53" t="n">
-        <v>5.723</v>
+        <v>5.921</v>
       </c>
       <c r="E53" t="n">
-        <v>3.793</v>
+        <v>0.6631</v>
       </c>
       <c r="F53" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54">
@@ -1498,16 +1498,16 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.8924</v>
+        <v>0.08048</v>
       </c>
       <c r="D54" t="n">
-        <v>5.521</v>
+        <v>5.491</v>
       </c>
       <c r="E54" t="n">
         <v>2.419</v>
       </c>
       <c r="F54" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55">
@@ -1518,16 +1518,16 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.04006</v>
+        <v>5.889e-19</v>
       </c>
       <c r="D55" t="n">
-        <v>5.256</v>
+        <v>6.233</v>
       </c>
       <c r="E55" t="n">
-        <v>7.908</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -1538,16 +1538,16 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.06797</v>
+        <v>0.002066</v>
       </c>
       <c r="D56" t="n">
-        <v>5.319</v>
+        <v>5.591</v>
       </c>
       <c r="E56" t="n">
         <v>5.223</v>
       </c>
       <c r="F56" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
@@ -1558,16 +1558,16 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.008366999999999999</v>
+        <v>0.3455</v>
       </c>
       <c r="D57" t="n">
-        <v>5.015</v>
+        <v>5.341</v>
       </c>
       <c r="E57" t="n">
-        <v>8.787000000000001</v>
+        <v>0.2023</v>
       </c>
       <c r="F57" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58">
@@ -1578,16 +1578,16 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>0.01629</v>
+        <v>0.4082</v>
       </c>
       <c r="D58" t="n">
-        <v>4.782</v>
+        <v>5.227</v>
       </c>
       <c r="E58" t="n">
-        <v>11.29</v>
+        <v>0.8213</v>
       </c>
       <c r="F58" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59">
@@ -1598,13 +1598,13 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.3051</v>
+        <v>0.4576</v>
       </c>
       <c r="D59" t="n">
-        <v>5.119</v>
+        <v>5.157</v>
       </c>
       <c r="E59" t="n">
-        <v>2.438</v>
+        <v>0.8869</v>
       </c>
       <c r="F59" t="n">
         <v>18</v>
@@ -1618,16 +1618,16 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>0.03417</v>
+        <v>5.74e-05</v>
       </c>
       <c r="D60" t="n">
-        <v>4.528</v>
+        <v>5.142</v>
       </c>
       <c r="E60" t="n">
         <v>5.903</v>
       </c>
       <c r="F60" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61">
@@ -1638,16 +1638,16 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>0.05077</v>
+        <v>0.01524</v>
       </c>
       <c r="D61" t="n">
-        <v>4.683</v>
+        <v>4.605</v>
       </c>
       <c r="E61" t="n">
         <v>0.2774</v>
       </c>
       <c r="F61" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -1658,16 +1658,16 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>0.147</v>
+        <v>0.03197</v>
       </c>
       <c r="D62" t="n">
-        <v>4.784</v>
+        <v>4.288</v>
       </c>
       <c r="E62" t="n">
         <v>1.055</v>
       </c>
       <c r="F62" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63">
@@ -1678,16 +1678,16 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>0.216</v>
+        <v>0.01792</v>
       </c>
       <c r="D63" t="n">
-        <v>4.747</v>
+        <v>4.276</v>
       </c>
       <c r="E63" t="n">
-        <v>2.31</v>
+        <v>2.296</v>
       </c>
       <c r="F63" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64">
@@ -1698,16 +1698,16 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>0.009783</v>
+        <v>8.577e-19</v>
       </c>
       <c r="D64" t="n">
-        <v>4.563</v>
+        <v>6.08</v>
       </c>
       <c r="E64" t="n">
-        <v>6.836</v>
+        <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
@@ -1718,16 +1718,16 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.005106</v>
+        <v>0.7052</v>
       </c>
       <c r="D65" t="n">
-        <v>5.132</v>
+        <v>10.28</v>
       </c>
       <c r="E65" t="n">
-        <v>6.556</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1738,16 +1738,16 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.02205</v>
+        <v>0.0009496</v>
       </c>
       <c r="D66" t="n">
-        <v>4.764</v>
+        <v>6.992</v>
       </c>
       <c r="E66" t="n">
         <v>5.25</v>
       </c>
       <c r="F66" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
@@ -1758,16 +1758,16 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>0.01528</v>
+        <v>0.01128</v>
       </c>
       <c r="D67" t="n">
-        <v>4.891</v>
+        <v>6.113</v>
       </c>
       <c r="E67" t="n">
         <v>3.808</v>
       </c>
       <c r="F67" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68">
@@ -1778,16 +1778,16 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1135</v>
+        <v>0.01327</v>
       </c>
       <c r="D68" t="n">
-        <v>4.952</v>
+        <v>5.244</v>
       </c>
       <c r="E68" t="n">
-        <v>3.493</v>
+        <v>3.092</v>
       </c>
       <c r="F68" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69">
@@ -1798,16 +1798,16 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1673</v>
+        <v>0.01674</v>
       </c>
       <c r="D69" t="n">
-        <v>4.934</v>
+        <v>5.044</v>
       </c>
       <c r="E69" t="n">
-        <v>1.581</v>
+        <v>0.1013</v>
       </c>
       <c r="F69" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70">
@@ -1818,16 +1818,16 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.02316</v>
+        <v>0.0002169</v>
       </c>
       <c r="D70" t="n">
-        <v>5.525</v>
+        <v>6.986</v>
       </c>
       <c r="E70" t="n">
         <v>2.211</v>
       </c>
       <c r="F70" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71">
@@ -1838,16 +1838,16 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.3763</v>
+        <v>0.08319</v>
       </c>
       <c r="D71" t="n">
-        <v>4.82</v>
+        <v>5.386</v>
       </c>
       <c r="E71" t="n">
-        <v>0.2145</v>
+        <v>0.6427</v>
       </c>
       <c r="F71" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72">
@@ -1858,16 +1858,16 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>0.02639</v>
+        <v>0.116</v>
       </c>
       <c r="D72" t="n">
-        <v>5.799</v>
+        <v>5.282</v>
       </c>
       <c r="E72" t="n">
-        <v>0.475</v>
+        <v>0.2679</v>
       </c>
       <c r="F72" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 05-14-2024 at 00:16
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -458,16 +458,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>7.16e-19</v>
+        <v>0.01244</v>
       </c>
       <c r="D2" t="n">
-        <v>1.352</v>
+        <v>0.8104</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.4966</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.39</v>
+        <v>0.1009</v>
       </c>
       <c r="D3" t="n">
-        <v>1.087</v>
+        <v>0.9441000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>8.346</v>
+        <v>0.09044000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -498,16 +498,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.403</v>
+        <v>0.3462</v>
       </c>
       <c r="D4" t="n">
-        <v>1.087</v>
+        <v>1.275</v>
       </c>
       <c r="E4" t="n">
-        <v>3.376</v>
+        <v>0.2749</v>
       </c>
       <c r="F4" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -518,16 +518,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4956</v>
+        <v>0.3308</v>
       </c>
       <c r="D5" t="n">
-        <v>1.283</v>
+        <v>0.968</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4391</v>
+        <v>0.1534</v>
       </c>
       <c r="F5" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3475</v>
+        <v>0.1351</v>
       </c>
       <c r="D6" t="n">
-        <v>1.216</v>
+        <v>1.069</v>
       </c>
       <c r="E6" t="n">
-        <v>1.154</v>
+        <v>0.1706</v>
       </c>
       <c r="F6" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -558,16 +558,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01168</v>
+        <v>0.1689</v>
       </c>
       <c r="D7" t="n">
-        <v>1.925</v>
+        <v>1.459</v>
       </c>
       <c r="E7" t="n">
-        <v>2.734</v>
+        <v>0.4461</v>
       </c>
       <c r="F7" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -578,16 +578,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7325</v>
+        <v>0.05829</v>
       </c>
       <c r="D8" t="n">
-        <v>1.411</v>
+        <v>1.546</v>
       </c>
       <c r="E8" t="n">
-        <v>4.85</v>
+        <v>1.399</v>
       </c>
       <c r="F8" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.07799</v>
+        <v>0.1939</v>
       </c>
       <c r="D9" t="n">
-        <v>2.249</v>
+        <v>2.099</v>
       </c>
       <c r="E9" t="n">
-        <v>8.132</v>
+        <v>0.2264</v>
       </c>
       <c r="F9" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -618,16 +618,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.165</v>
+        <v>0.4062</v>
       </c>
       <c r="D10" t="n">
-        <v>1.887</v>
+        <v>1.925</v>
       </c>
       <c r="E10" t="n">
-        <v>8.157</v>
+        <v>0.2214</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -638,16 +638,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.158</v>
+        <v>0.4228</v>
       </c>
       <c r="D11" t="n">
-        <v>1.893</v>
+        <v>1.793</v>
       </c>
       <c r="E11" t="n">
-        <v>1.981</v>
+        <v>0.1071</v>
       </c>
       <c r="F11" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
@@ -658,16 +658,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2192</v>
+        <v>0.0965</v>
       </c>
       <c r="D12" t="n">
-        <v>1.961</v>
+        <v>1.893</v>
       </c>
       <c r="E12" t="n">
-        <v>5.746</v>
+        <v>0.2045</v>
       </c>
       <c r="F12" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -678,16 +678,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.244</v>
+        <v>0.002187</v>
       </c>
       <c r="D13" t="n">
-        <v>2.067</v>
+        <v>2.011</v>
       </c>
       <c r="E13" t="n">
         <v>0.1693</v>
       </c>
       <c r="F13" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -698,16 +698,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2771</v>
+        <v>0.1009</v>
       </c>
       <c r="D14" t="n">
-        <v>2.147</v>
+        <v>2.41</v>
       </c>
       <c r="E14" t="n">
-        <v>1.517</v>
+        <v>0.3006</v>
       </c>
       <c r="F14" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -718,16 +718,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8951</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>1.877</v>
+        <v>2.553</v>
       </c>
       <c r="E15" t="n">
-        <v>2.119</v>
+        <v>0.242</v>
       </c>
       <c r="F15" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -738,16 +738,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.00134</v>
+        <v>0.1088</v>
       </c>
       <c r="D16" t="n">
-        <v>2.986</v>
+        <v>2.786</v>
       </c>
       <c r="E16" t="n">
-        <v>0.7079</v>
+        <v>0.5896</v>
       </c>
       <c r="F16" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
@@ -758,16 +758,16 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>8.933000000000001e-19</v>
+        <v>0.0002662</v>
       </c>
       <c r="D17" t="n">
-        <v>4.673</v>
+        <v>2.895</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.2886</v>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -778,16 +778,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.003378</v>
+        <v>0.007861</v>
       </c>
       <c r="D18" t="n">
-        <v>3.301</v>
+        <v>3.097</v>
       </c>
       <c r="E18" t="n">
-        <v>1.842</v>
+        <v>0.2737</v>
       </c>
       <c r="F18" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -798,16 +798,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0537</v>
+        <v>0.1738</v>
       </c>
       <c r="D19" t="n">
-        <v>2.855</v>
+        <v>2.905</v>
       </c>
       <c r="E19" t="n">
-        <v>1.833</v>
+        <v>0.2202</v>
       </c>
       <c r="F19" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
@@ -818,16 +818,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.03501</v>
+        <v>0.01252</v>
       </c>
       <c r="D20" t="n">
-        <v>3.166</v>
+        <v>3.328</v>
       </c>
       <c r="E20" t="n">
-        <v>3.975</v>
+        <v>0.1245</v>
       </c>
       <c r="F20" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -838,16 +838,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.03476</v>
+        <v>0.0126</v>
       </c>
       <c r="D21" t="n">
-        <v>3.315</v>
+        <v>3.479</v>
       </c>
       <c r="E21" t="n">
-        <v>2.251</v>
+        <v>0.107</v>
       </c>
       <c r="F21" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -858,13 +858,13 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.03365</v>
+        <v>0.001719</v>
       </c>
       <c r="D22" t="n">
-        <v>3.471</v>
+        <v>3.94</v>
       </c>
       <c r="E22" t="n">
-        <v>2.27</v>
+        <v>0.105</v>
       </c>
       <c r="F22" t="n">
         <v>12</v>
@@ -878,16 +878,16 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.07542</v>
+        <v>0.0002045</v>
       </c>
       <c r="D23" t="n">
-        <v>3.46</v>
+        <v>4.967</v>
       </c>
       <c r="E23" t="n">
-        <v>2.956</v>
+        <v>0.3142</v>
       </c>
       <c r="F23" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
@@ -898,16 +898,16 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1338</v>
+        <v>0.004486</v>
       </c>
       <c r="D24" t="n">
-        <v>3.465</v>
+        <v>4.275</v>
       </c>
       <c r="E24" t="n">
-        <v>1.083</v>
+        <v>0.4583</v>
       </c>
       <c r="F24" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25">
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1851</v>
+        <v>0.001384</v>
       </c>
       <c r="D25" t="n">
-        <v>3.375</v>
+        <v>5.265</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6208</v>
+        <v>0.3796</v>
       </c>
       <c r="F25" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -938,16 +938,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.429</v>
+        <v>0.0008876999999999999</v>
       </c>
       <c r="D26" t="n">
-        <v>7.131</v>
+        <v>5.509</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>0.1375</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
@@ -958,16 +958,16 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>1.262e-29</v>
+        <v>0.006732</v>
       </c>
       <c r="D27" t="n">
-        <v>6.608</v>
+        <v>4.791</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>0.2124</v>
       </c>
       <c r="F27" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
@@ -978,16 +978,16 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.001944</v>
+        <v>0.01462</v>
       </c>
       <c r="D28" t="n">
-        <v>5.613</v>
+        <v>5.022</v>
       </c>
       <c r="E28" t="n">
-        <v>1.064</v>
+        <v>0.06677</v>
       </c>
       <c r="F28" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29">
@@ -998,16 +998,16 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.002924</v>
+        <v>0.0009169</v>
       </c>
       <c r="D29" t="n">
-        <v>5.429</v>
+        <v>4.787</v>
       </c>
       <c r="E29" t="n">
-        <v>2.841</v>
+        <v>0.04599</v>
       </c>
       <c r="F29" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -1018,16 +1018,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.2944</v>
+        <v>0.0001061</v>
       </c>
       <c r="D30" t="n">
-        <v>8.938000000000001</v>
+        <v>5.315</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>0.07238</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -1038,16 +1038,16 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01533</v>
+        <v>0.06807000000000001</v>
       </c>
       <c r="D31" t="n">
-        <v>5.019</v>
+        <v>4.74</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9826</v>
+        <v>0.253</v>
       </c>
       <c r="F31" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
@@ -1058,16 +1058,16 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1035</v>
+        <v>9.308e-06</v>
       </c>
       <c r="D32" t="n">
-        <v>4.556</v>
+        <v>5.487</v>
       </c>
       <c r="E32" t="n">
-        <v>0.764</v>
+        <v>0.3387</v>
       </c>
       <c r="F32" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
@@ -1078,16 +1078,16 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0824</v>
+        <v>0.01389</v>
       </c>
       <c r="D33" t="n">
-        <v>4.61</v>
+        <v>5.046</v>
       </c>
       <c r="E33" t="n">
-        <v>1.01</v>
+        <v>0.2695</v>
       </c>
       <c r="F33" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
@@ -1098,16 +1098,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1264</v>
+        <v>0.001119</v>
       </c>
       <c r="D34" t="n">
-        <v>4.457</v>
+        <v>4.833</v>
       </c>
       <c r="E34" t="n">
-        <v>0.301</v>
+        <v>0.04521</v>
       </c>
       <c r="F34" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
@@ -1118,16 +1118,16 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.104</v>
+        <v>0.001326</v>
       </c>
       <c r="D35" t="n">
-        <v>4.554</v>
+        <v>4.945</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6122</v>
+        <v>0.164</v>
       </c>
       <c r="F35" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36">
@@ -1138,16 +1138,16 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>2.312e-19</v>
+        <v>2.998e-29</v>
       </c>
       <c r="D36" t="n">
-        <v>7.081</v>
+        <v>6.24</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.1078</v>
       </c>
       <c r="F36" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -1158,16 +1158,16 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.01241</v>
+        <v>0.05605</v>
       </c>
       <c r="D37" t="n">
-        <v>5.121</v>
+        <v>5.25</v>
       </c>
       <c r="E37" t="n">
-        <v>3.407</v>
+        <v>0.0853</v>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38">
@@ -1178,16 +1178,16 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.04219</v>
+        <v>0.001069</v>
       </c>
       <c r="D38" t="n">
-        <v>5.038</v>
+        <v>5.933</v>
       </c>
       <c r="E38" t="n">
-        <v>0.8683999999999999</v>
+        <v>0.1564</v>
       </c>
       <c r="F38" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -1198,16 +1198,16 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.03904</v>
+        <v>0.004094</v>
       </c>
       <c r="D39" t="n">
-        <v>5.085</v>
+        <v>5.513</v>
       </c>
       <c r="E39" t="n">
-        <v>0.552</v>
+        <v>0.5288</v>
       </c>
       <c r="F39" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40">
@@ -1218,16 +1218,16 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.06263000000000001</v>
+        <v>0.01848</v>
       </c>
       <c r="D40" t="n">
-        <v>5.082</v>
+        <v>5.432</v>
       </c>
       <c r="E40" t="n">
-        <v>1.165</v>
+        <v>0.2089</v>
       </c>
       <c r="F40" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -1238,16 +1238,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1733</v>
+        <v>0.006495</v>
       </c>
       <c r="D41" t="n">
-        <v>4.953</v>
+        <v>5.426</v>
       </c>
       <c r="E41" t="n">
-        <v>0.07194</v>
+        <v>0.08316999999999999</v>
       </c>
       <c r="F41" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42">
@@ -1258,16 +1258,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.00175</v>
+        <v>0.006423</v>
       </c>
       <c r="D42" t="n">
-        <v>5.667</v>
+        <v>5.554</v>
       </c>
       <c r="E42" t="n">
-        <v>0.6876</v>
+        <v>0.2838</v>
       </c>
       <c r="F42" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
@@ -1278,16 +1278,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.02719</v>
+        <v>0.1434</v>
       </c>
       <c r="D43" t="n">
-        <v>5.177</v>
+        <v>5.236</v>
       </c>
       <c r="E43" t="n">
-        <v>5.025</v>
+        <v>0.2819</v>
       </c>
       <c r="F43" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44">
@@ -1298,16 +1298,16 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.6196</v>
+        <v>1.231e-28</v>
       </c>
       <c r="D44" t="n">
-        <v>5.13</v>
+        <v>6.423</v>
       </c>
       <c r="E44" t="n">
-        <v>5.344</v>
+        <v>0.7166</v>
       </c>
       <c r="F44" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45">
@@ -1318,16 +1318,16 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.5965</v>
+        <v>0.048</v>
       </c>
       <c r="D45" t="n">
-        <v>5.141</v>
+        <v>5.488</v>
       </c>
       <c r="E45" t="n">
-        <v>2.722</v>
+        <v>1.173</v>
       </c>
       <c r="F45" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46">
@@ -1338,16 +1338,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.00479</v>
+        <v>0.1221</v>
       </c>
       <c r="D46" t="n">
-        <v>6.554</v>
+        <v>5.687</v>
       </c>
       <c r="E46" t="n">
-        <v>5.745</v>
+        <v>0.4614</v>
       </c>
       <c r="F46" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47">
@@ -1358,16 +1358,16 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.06633</v>
+        <v>0.3026</v>
       </c>
       <c r="D47" t="n">
-        <v>5.719</v>
+        <v>5.804</v>
       </c>
       <c r="E47" t="n">
-        <v>1.158</v>
+        <v>0.07955</v>
       </c>
       <c r="F47" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
@@ -1378,16 +1378,16 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>1.252e-19</v>
+        <v>0.02337</v>
       </c>
       <c r="D48" t="n">
-        <v>7.863</v>
+        <v>5.823</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>0.06987</v>
       </c>
       <c r="F48" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49">
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1792</v>
+        <v>0.02265</v>
       </c>
       <c r="D49" t="n">
-        <v>5.803</v>
+        <v>5.867</v>
       </c>
       <c r="E49" t="n">
-        <v>0.9627</v>
+        <v>0.4875</v>
       </c>
       <c r="F49" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50">
@@ -1418,16 +1418,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>1.037</v>
+        <v>0.03538</v>
       </c>
       <c r="D50" t="n">
-        <v>5.371</v>
+        <v>5.914</v>
       </c>
       <c r="E50" t="n">
         <v>1.27</v>
       </c>
       <c r="F50" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51">
@@ -1438,16 +1438,16 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>1.367</v>
+        <v>0.003351</v>
       </c>
       <c r="D51" t="n">
-        <v>9.071</v>
+        <v>6.443</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>0.6151</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1458,16 +1458,16 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>1.349e-18</v>
+        <v>0.03072</v>
       </c>
       <c r="D52" t="n">
-        <v>7.858</v>
+        <v>5.697</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>0.4801</v>
       </c>
       <c r="F52" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53">
@@ -1478,16 +1478,16 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>0.03151</v>
+        <v>0.08151</v>
       </c>
       <c r="D53" t="n">
-        <v>5.921</v>
+        <v>5.87</v>
       </c>
       <c r="E53" t="n">
-        <v>0.6631</v>
+        <v>0.3352</v>
       </c>
       <c r="F53" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54">
@@ -1498,16 +1498,16 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>0.08048</v>
+        <v>0.6843</v>
       </c>
       <c r="D54" t="n">
-        <v>5.491</v>
+        <v>5.576</v>
       </c>
       <c r="E54" t="n">
-        <v>2.419</v>
+        <v>0.4235</v>
       </c>
       <c r="F54" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55">
@@ -1518,16 +1518,16 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>5.889e-19</v>
+        <v>0.008108000000000001</v>
       </c>
       <c r="D55" t="n">
-        <v>6.233</v>
+        <v>4.895</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>0.1901</v>
       </c>
       <c r="F55" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56">
@@ -1538,16 +1538,16 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>0.002066</v>
+        <v>0.07369000000000001</v>
       </c>
       <c r="D56" t="n">
-        <v>5.591</v>
+        <v>5.145</v>
       </c>
       <c r="E56" t="n">
-        <v>5.223</v>
+        <v>0.1319</v>
       </c>
       <c r="F56" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57">
@@ -1558,16 +1558,16 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.3455</v>
+        <v>0.007827000000000001</v>
       </c>
       <c r="D57" t="n">
-        <v>5.341</v>
+        <v>4.831</v>
       </c>
       <c r="E57" t="n">
-        <v>0.2023</v>
+        <v>0.5063</v>
       </c>
       <c r="F57" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58">
@@ -1578,16 +1578,16 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>0.4082</v>
+        <v>0.01284</v>
       </c>
       <c r="D58" t="n">
-        <v>5.227</v>
+        <v>4.479</v>
       </c>
       <c r="E58" t="n">
-        <v>0.8213</v>
+        <v>0.361</v>
       </c>
       <c r="F58" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59">
@@ -1598,16 +1598,16 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.4576</v>
+        <v>0.2662</v>
       </c>
       <c r="D59" t="n">
-        <v>5.157</v>
+        <v>5.16</v>
       </c>
       <c r="E59" t="n">
-        <v>0.8869</v>
+        <v>0.09773999999999999</v>
       </c>
       <c r="F59" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60">
@@ -1618,16 +1618,16 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>5.74e-05</v>
+        <v>0.02578</v>
       </c>
       <c r="D60" t="n">
-        <v>5.142</v>
+        <v>4.62</v>
       </c>
       <c r="E60" t="n">
-        <v>5.903</v>
+        <v>0.07553</v>
       </c>
       <c r="F60" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61">
@@ -1638,16 +1638,16 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>0.01524</v>
+        <v>0.04162</v>
       </c>
       <c r="D61" t="n">
-        <v>4.605</v>
+        <v>4.699</v>
       </c>
       <c r="E61" t="n">
-        <v>0.2774</v>
+        <v>0.124</v>
       </c>
       <c r="F61" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62">
@@ -1658,16 +1658,16 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>0.03197</v>
+        <v>0.1212</v>
       </c>
       <c r="D62" t="n">
-        <v>4.288</v>
+        <v>4.882</v>
       </c>
       <c r="E62" t="n">
-        <v>1.055</v>
+        <v>0.1589</v>
       </c>
       <c r="F62" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63">
@@ -1678,16 +1678,16 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>0.01792</v>
+        <v>0.1728</v>
       </c>
       <c r="D63" t="n">
-        <v>4.276</v>
+        <v>4.809</v>
       </c>
       <c r="E63" t="n">
-        <v>2.296</v>
+        <v>0.9268999999999999</v>
       </c>
       <c r="F63" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64">
@@ -1698,16 +1698,16 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>8.577e-19</v>
+        <v>0.006985</v>
       </c>
       <c r="D64" t="n">
-        <v>6.08</v>
+        <v>4.325</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>0.2466</v>
       </c>
       <c r="F64" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65">
@@ -1718,16 +1718,16 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.7052</v>
+        <v>0.004142</v>
       </c>
       <c r="D65" t="n">
-        <v>10.28</v>
+        <v>5.26</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>0.2186</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -1738,16 +1738,16 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.0009496</v>
+        <v>0.01208</v>
       </c>
       <c r="D66" t="n">
-        <v>6.992</v>
+        <v>5.06</v>
       </c>
       <c r="E66" t="n">
-        <v>5.25</v>
+        <v>1.013</v>
       </c>
       <c r="F66" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67">
@@ -1758,16 +1758,16 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>0.01128</v>
+        <v>0.01316</v>
       </c>
       <c r="D67" t="n">
-        <v>6.113</v>
+        <v>5.189</v>
       </c>
       <c r="E67" t="n">
-        <v>3.808</v>
+        <v>0.177</v>
       </c>
       <c r="F67" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68">
@@ -1778,16 +1778,16 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.01327</v>
+        <v>0.08619</v>
       </c>
       <c r="D68" t="n">
-        <v>5.244</v>
+        <v>5.176</v>
       </c>
       <c r="E68" t="n">
-        <v>3.092</v>
+        <v>0.1181</v>
       </c>
       <c r="F68" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69">
@@ -1798,16 +1798,16 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>0.01674</v>
+        <v>0.006925</v>
       </c>
       <c r="D69" t="n">
-        <v>5.044</v>
+        <v>5.872</v>
       </c>
       <c r="E69" t="n">
         <v>0.1013</v>
       </c>
       <c r="F69" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70">
@@ -1818,16 +1818,16 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>0.0002169</v>
+        <v>0.02144</v>
       </c>
       <c r="D70" t="n">
-        <v>6.986</v>
+        <v>5.9</v>
       </c>
       <c r="E70" t="n">
-        <v>2.211</v>
+        <v>0.0873</v>
       </c>
       <c r="F70" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71">
@@ -1838,16 +1838,16 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.08319</v>
+        <v>0.01113</v>
       </c>
       <c r="D71" t="n">
-        <v>5.386</v>
+        <v>6.014</v>
       </c>
       <c r="E71" t="n">
-        <v>0.6427</v>
+        <v>0.2145</v>
       </c>
       <c r="F71" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72">
@@ -1858,16 +1858,16 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>0.116</v>
+        <v>0.02255</v>
       </c>
       <c r="D72" t="n">
-        <v>5.282</v>
+        <v>6.167</v>
       </c>
       <c r="E72" t="n">
-        <v>0.2679</v>
+        <v>0.1816</v>
       </c>
       <c r="F72" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 05-15-2024 at 18:20
</commit_message>
<xml_diff>
--- a/experiment_2/output/output_covid_hard.xlsx
+++ b/experiment_2/output/output_covid_hard.xlsx
@@ -458,16 +458,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01244</v>
+        <v>2.473e-19</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8104</v>
+        <v>1.602</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4966</v>
+        <v>0.526</v>
       </c>
       <c r="F2" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1009</v>
+        <v>1.81e-18</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9441000000000001</v>
+        <v>1.995</v>
       </c>
       <c r="E3" t="n">
-        <v>0.09044000000000001</v>
+        <v>0.5928</v>
       </c>
       <c r="F3" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -501,13 +501,13 @@
         <v>0.3462</v>
       </c>
       <c r="D4" t="n">
-        <v>1.275</v>
+        <v>1.112</v>
       </c>
       <c r="E4" t="n">
         <v>0.2749</v>
       </c>
       <c r="F4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -521,13 +521,13 @@
         <v>0.3308</v>
       </c>
       <c r="D5" t="n">
-        <v>0.968</v>
+        <v>0.6518</v>
       </c>
       <c r="E5" t="n">
         <v>0.1534</v>
       </c>
       <c r="F5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -541,13 +541,13 @@
         <v>0.1351</v>
       </c>
       <c r="D6" t="n">
-        <v>1.069</v>
+        <v>0.7959000000000001</v>
       </c>
       <c r="E6" t="n">
         <v>0.1706</v>
       </c>
       <c r="F6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -558,16 +558,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1689</v>
+        <v>0.06888</v>
       </c>
       <c r="D7" t="n">
-        <v>1.459</v>
+        <v>1.33</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4461</v>
+        <v>0.4627</v>
       </c>
       <c r="F7" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>0.05829</v>
       </c>
       <c r="D8" t="n">
-        <v>1.546</v>
+        <v>1.523</v>
       </c>
       <c r="E8" t="n">
         <v>1.399</v>
       </c>
       <c r="F8" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1939</v>
+        <v>0.2477</v>
       </c>
       <c r="D9" t="n">
-        <v>2.099</v>
+        <v>1.86</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2264</v>
+        <v>1.228</v>
       </c>
       <c r="F9" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -618,16 +618,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4062</v>
+        <v>0.4646</v>
       </c>
       <c r="D10" t="n">
-        <v>1.925</v>
+        <v>1.368</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2214</v>
+        <v>0.5923</v>
       </c>
       <c r="F10" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -641,13 +641,13 @@
         <v>0.4228</v>
       </c>
       <c r="D11" t="n">
-        <v>1.793</v>
+        <v>1.505</v>
       </c>
       <c r="E11" t="n">
         <v>0.1071</v>
       </c>
       <c r="F11" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -658,16 +658,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0965</v>
+        <v>0.3204</v>
       </c>
       <c r="D12" t="n">
-        <v>1.893</v>
+        <v>1.641</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2045</v>
+        <v>0.7953</v>
       </c>
       <c r="F12" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -681,13 +681,13 @@
         <v>0.002187</v>
       </c>
       <c r="D13" t="n">
-        <v>2.011</v>
+        <v>1.546</v>
       </c>
       <c r="E13" t="n">
         <v>0.1693</v>
       </c>
       <c r="F13" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -701,13 +701,13 @@
         <v>0.1009</v>
       </c>
       <c r="D14" t="n">
-        <v>2.41</v>
+        <v>2.353</v>
       </c>
       <c r="E14" t="n">
         <v>0.3006</v>
       </c>
       <c r="F14" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
@@ -721,13 +721,13 @@
         <v>0.09429999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>2.553</v>
+        <v>2.451</v>
       </c>
       <c r="E15" t="n">
         <v>0.242</v>
       </c>
       <c r="F15" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -738,16 +738,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1088</v>
+        <v>0.00134</v>
       </c>
       <c r="D16" t="n">
-        <v>2.786</v>
+        <v>2.062</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5896</v>
+        <v>0.7192</v>
       </c>
       <c r="F16" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -761,13 +761,13 @@
         <v>0.0002662</v>
       </c>
       <c r="D17" t="n">
-        <v>2.895</v>
+        <v>2.281</v>
       </c>
       <c r="E17" t="n">
         <v>0.2886</v>
       </c>
       <c r="F17" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -781,13 +781,13 @@
         <v>0.007861</v>
       </c>
       <c r="D18" t="n">
-        <v>3.097</v>
+        <v>2.941</v>
       </c>
       <c r="E18" t="n">
         <v>0.2737</v>
       </c>
       <c r="F18" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
@@ -801,13 +801,13 @@
         <v>0.1738</v>
       </c>
       <c r="D19" t="n">
-        <v>2.905</v>
+        <v>2.607</v>
       </c>
       <c r="E19" t="n">
         <v>0.2202</v>
       </c>
       <c r="F19" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
@@ -818,16 +818,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01252</v>
+        <v>0.01123</v>
       </c>
       <c r="D20" t="n">
-        <v>3.328</v>
+        <v>3.101</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1245</v>
+        <v>0.2173</v>
       </c>
       <c r="F20" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
@@ -841,13 +841,13 @@
         <v>0.0126</v>
       </c>
       <c r="D21" t="n">
-        <v>3.479</v>
+        <v>3.25</v>
       </c>
       <c r="E21" t="n">
         <v>0.107</v>
       </c>
       <c r="F21" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -858,16 +858,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.001719</v>
+        <v>0.008581999999999999</v>
       </c>
       <c r="D22" t="n">
-        <v>3.94</v>
+        <v>3.206</v>
       </c>
       <c r="E22" t="n">
-        <v>0.105</v>
+        <v>0.1225</v>
       </c>
       <c r="F22" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
@@ -878,16 +878,16 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0002045</v>
+        <v>0.03624</v>
       </c>
       <c r="D23" t="n">
-        <v>4.967</v>
+        <v>3.094</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3142</v>
+        <v>0.4257</v>
       </c>
       <c r="F23" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -898,16 +898,16 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.004486</v>
+        <v>0.01635</v>
       </c>
       <c r="D24" t="n">
-        <v>4.275</v>
+        <v>3.287</v>
       </c>
       <c r="E24" t="n">
-        <v>0.4583</v>
+        <v>0.6127</v>
       </c>
       <c r="F24" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25">
@@ -918,16 +918,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.001384</v>
+        <v>0.009377</v>
       </c>
       <c r="D25" t="n">
-        <v>5.265</v>
+        <v>3.895</v>
       </c>
       <c r="E25" t="n">
-        <v>0.3796</v>
+        <v>0.6296</v>
       </c>
       <c r="F25" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
@@ -938,16 +938,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0008876999999999999</v>
+        <v>0.01314</v>
       </c>
       <c r="D26" t="n">
-        <v>5.509</v>
+        <v>3.782</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1375</v>
+        <v>0.1966</v>
       </c>
       <c r="F26" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
@@ -958,16 +958,16 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.006732</v>
+        <v>0.01183</v>
       </c>
       <c r="D27" t="n">
-        <v>4.791</v>
+        <v>4.497</v>
       </c>
       <c r="E27" t="n">
-        <v>0.2124</v>
+        <v>0.3537</v>
       </c>
       <c r="F27" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
@@ -978,16 +978,16 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01462</v>
+        <v>0.0006742</v>
       </c>
       <c r="D28" t="n">
-        <v>5.022</v>
+        <v>4.164</v>
       </c>
       <c r="E28" t="n">
-        <v>0.06677</v>
+        <v>0.526</v>
       </c>
       <c r="F28" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -998,16 +998,16 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0009169</v>
+        <v>0.02656</v>
       </c>
       <c r="D29" t="n">
-        <v>4.787</v>
+        <v>4.59</v>
       </c>
       <c r="E29" t="n">
-        <v>0.04599</v>
+        <v>0.1488</v>
       </c>
       <c r="F29" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30">
@@ -1018,16 +1018,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0001061</v>
+        <v>0.0008779</v>
       </c>
       <c r="D30" t="n">
-        <v>5.315</v>
+        <v>4.464</v>
       </c>
       <c r="E30" t="n">
-        <v>0.07238</v>
+        <v>0.2842</v>
       </c>
       <c r="F30" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
@@ -1041,13 +1041,13 @@
         <v>0.06807000000000001</v>
       </c>
       <c r="D31" t="n">
-        <v>4.74</v>
+        <v>4.294</v>
       </c>
       <c r="E31" t="n">
         <v>0.253</v>
       </c>
       <c r="F31" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32">
@@ -1058,16 +1058,16 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>9.308e-06</v>
+        <v>0.0004758</v>
       </c>
       <c r="D32" t="n">
-        <v>5.487</v>
+        <v>3.839</v>
       </c>
       <c r="E32" t="n">
-        <v>0.3387</v>
+        <v>0.6179</v>
       </c>
       <c r="F32" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33">
@@ -1081,13 +1081,13 @@
         <v>0.01389</v>
       </c>
       <c r="D33" t="n">
-        <v>5.046</v>
+        <v>4.602</v>
       </c>
       <c r="E33" t="n">
         <v>0.2695</v>
       </c>
       <c r="F33" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
@@ -1098,16 +1098,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.001119</v>
+        <v>0.005308</v>
       </c>
       <c r="D34" t="n">
-        <v>4.833</v>
+        <v>4.643</v>
       </c>
       <c r="E34" t="n">
-        <v>0.04521</v>
+        <v>0.3045</v>
       </c>
       <c r="F34" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35">
@@ -1121,13 +1121,13 @@
         <v>0.001326</v>
       </c>
       <c r="D35" t="n">
-        <v>4.945</v>
+        <v>4.502</v>
       </c>
       <c r="E35" t="n">
         <v>0.164</v>
       </c>
       <c r="F35" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
@@ -1138,16 +1138,16 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>2.998e-29</v>
+        <v>0.0005083</v>
       </c>
       <c r="D36" t="n">
-        <v>6.24</v>
+        <v>4.651</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1078</v>
+        <v>0.2042</v>
       </c>
       <c r="F36" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37">
@@ -1158,16 +1158,16 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.05605</v>
+        <v>0.07881000000000001</v>
       </c>
       <c r="D37" t="n">
-        <v>5.25</v>
+        <v>4.605</v>
       </c>
       <c r="E37" t="n">
-        <v>0.0853</v>
+        <v>0.2847</v>
       </c>
       <c r="F37" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38">
@@ -1178,16 +1178,16 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.001069</v>
+        <v>0.06856</v>
       </c>
       <c r="D38" t="n">
-        <v>5.933</v>
+        <v>4.639</v>
       </c>
       <c r="E38" t="n">
-        <v>0.1564</v>
+        <v>0.4637</v>
       </c>
       <c r="F38" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39">
@@ -1198,16 +1198,16 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.004094</v>
+        <v>0.03904</v>
       </c>
       <c r="D39" t="n">
-        <v>5.513</v>
+        <v>4.673</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5288</v>
+        <v>0.7395</v>
       </c>
       <c r="F39" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40">
@@ -1221,13 +1221,13 @@
         <v>0.01848</v>
       </c>
       <c r="D40" t="n">
-        <v>5.432</v>
+        <v>4.985</v>
       </c>
       <c r="E40" t="n">
         <v>0.2089</v>
       </c>
       <c r="F40" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41">
@@ -1241,13 +1241,13 @@
         <v>0.006495</v>
       </c>
       <c r="D41" t="n">
-        <v>5.426</v>
+        <v>4.989</v>
       </c>
       <c r="E41" t="n">
         <v>0.08316999999999999</v>
       </c>
       <c r="F41" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42">
@@ -1258,16 +1258,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.006423</v>
+        <v>0.003861</v>
       </c>
       <c r="D42" t="n">
-        <v>5.554</v>
+        <v>4.937</v>
       </c>
       <c r="E42" t="n">
-        <v>0.2838</v>
+        <v>0.3786</v>
       </c>
       <c r="F42" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
@@ -1281,13 +1281,13 @@
         <v>0.1434</v>
       </c>
       <c r="D43" t="n">
-        <v>5.236</v>
+        <v>4.774</v>
       </c>
       <c r="E43" t="n">
         <v>0.2819</v>
       </c>
       <c r="F43" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44">
@@ -1298,16 +1298,16 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>1.231e-28</v>
+        <v>0.229</v>
       </c>
       <c r="D44" t="n">
-        <v>6.423</v>
+        <v>4.86</v>
       </c>
       <c r="E44" t="n">
-        <v>0.7166</v>
+        <v>1.989</v>
       </c>
       <c r="F44" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45">
@@ -1318,16 +1318,16 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.048</v>
+        <v>0.01825</v>
       </c>
       <c r="D45" t="n">
-        <v>5.488</v>
+        <v>4.494</v>
       </c>
       <c r="E45" t="n">
-        <v>1.173</v>
+        <v>2.31</v>
       </c>
       <c r="F45" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
@@ -1341,13 +1341,13 @@
         <v>0.1221</v>
       </c>
       <c r="D46" t="n">
-        <v>5.687</v>
+        <v>5.243</v>
       </c>
       <c r="E46" t="n">
         <v>0.4614</v>
       </c>
       <c r="F46" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47">
@@ -1358,16 +1358,16 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.3026</v>
+        <v>0.2315</v>
       </c>
       <c r="D47" t="n">
-        <v>5.804</v>
+        <v>5.416</v>
       </c>
       <c r="E47" t="n">
-        <v>0.07955</v>
+        <v>0.6021</v>
       </c>
       <c r="F47" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48">
@@ -1378,16 +1378,16 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>0.02337</v>
+        <v>0.406</v>
       </c>
       <c r="D48" t="n">
-        <v>5.823</v>
+        <v>5.153</v>
       </c>
       <c r="E48" t="n">
-        <v>0.06987</v>
+        <v>0.144</v>
       </c>
       <c r="F48" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49">
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.02265</v>
+        <v>1.754e-18</v>
       </c>
       <c r="D49" t="n">
-        <v>5.867</v>
+        <v>6.09</v>
       </c>
       <c r="E49" t="n">
-        <v>0.4875</v>
+        <v>0.5756</v>
       </c>
       <c r="F49" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -1418,16 +1418,16 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.03538</v>
+        <v>0.03743</v>
       </c>
       <c r="D50" t="n">
-        <v>5.914</v>
+        <v>5.558</v>
       </c>
       <c r="E50" t="n">
-        <v>1.27</v>
+        <v>1.615</v>
       </c>
       <c r="F50" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51">
@@ -1438,16 +1438,16 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>0.003351</v>
+        <v>1.261e-17</v>
       </c>
       <c r="D51" t="n">
-        <v>6.443</v>
+        <v>5.469</v>
       </c>
       <c r="E51" t="n">
-        <v>0.6151</v>
+        <v>0.9634</v>
       </c>
       <c r="F51" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -1458,16 +1458,16 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>0.03072</v>
+        <v>0.02474</v>
       </c>
       <c r="D52" t="n">
-        <v>5.697</v>
+        <v>5.327</v>
       </c>
       <c r="E52" t="n">
-        <v>0.4801</v>
+        <v>1.329</v>
       </c>
       <c r="F52" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53">
@@ -1481,13 +1481,13 @@
         <v>0.08151</v>
       </c>
       <c r="D53" t="n">
-        <v>5.87</v>
+        <v>5.445</v>
       </c>
       <c r="E53" t="n">
         <v>0.3352</v>
       </c>
       <c r="F53" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54">
@@ -1501,13 +1501,13 @@
         <v>0.6843</v>
       </c>
       <c r="D54" t="n">
-        <v>5.576</v>
+        <v>5.093</v>
       </c>
       <c r="E54" t="n">
         <v>0.4235</v>
       </c>
       <c r="F54" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55">
@@ -1518,16 +1518,16 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.008108000000000001</v>
+        <v>0.3566</v>
       </c>
       <c r="D55" t="n">
-        <v>4.895</v>
+        <v>5.026</v>
       </c>
       <c r="E55" t="n">
-        <v>0.1901</v>
+        <v>1.096</v>
       </c>
       <c r="F55" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56">
@@ -1541,13 +1541,13 @@
         <v>0.07369000000000001</v>
       </c>
       <c r="D56" t="n">
-        <v>5.145</v>
+        <v>4.767</v>
       </c>
       <c r="E56" t="n">
         <v>0.1319</v>
       </c>
       <c r="F56" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57">
@@ -1558,16 +1558,16 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>0.007827000000000001</v>
+        <v>0.02181</v>
       </c>
       <c r="D57" t="n">
-        <v>4.831</v>
+        <v>4.609</v>
       </c>
       <c r="E57" t="n">
-        <v>0.5063</v>
+        <v>0.6167</v>
       </c>
       <c r="F57" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58">
@@ -1581,13 +1581,13 @@
         <v>0.01284</v>
       </c>
       <c r="D58" t="n">
-        <v>4.479</v>
+        <v>3.524</v>
       </c>
       <c r="E58" t="n">
         <v>0.361</v>
       </c>
       <c r="F58" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59">
@@ -1598,16 +1598,16 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>0.2662</v>
+        <v>0.243</v>
       </c>
       <c r="D59" t="n">
-        <v>5.16</v>
+        <v>4.662</v>
       </c>
       <c r="E59" t="n">
-        <v>0.09773999999999999</v>
+        <v>0.3571</v>
       </c>
       <c r="F59" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60">
@@ -1621,13 +1621,13 @@
         <v>0.02578</v>
       </c>
       <c r="D60" t="n">
-        <v>4.62</v>
+        <v>4.212</v>
       </c>
       <c r="E60" t="n">
         <v>0.07553</v>
       </c>
       <c r="F60" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61">
@@ -1638,16 +1638,16 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>0.04162</v>
+        <v>0.194</v>
       </c>
       <c r="D61" t="n">
-        <v>4.699</v>
+        <v>4.492</v>
       </c>
       <c r="E61" t="n">
-        <v>0.124</v>
+        <v>0.1818</v>
       </c>
       <c r="F61" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62">
@@ -1658,16 +1658,16 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1212</v>
+        <v>0.147</v>
       </c>
       <c r="D62" t="n">
-        <v>4.882</v>
+        <v>4.398</v>
       </c>
       <c r="E62" t="n">
-        <v>0.1589</v>
+        <v>0.1987</v>
       </c>
       <c r="F62" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63">
@@ -1681,13 +1681,13 @@
         <v>0.1728</v>
       </c>
       <c r="D63" t="n">
-        <v>4.809</v>
+        <v>4.4</v>
       </c>
       <c r="E63" t="n">
         <v>0.9268999999999999</v>
       </c>
       <c r="F63" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64">
@@ -1698,16 +1698,16 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>0.006985</v>
+        <v>0.006758</v>
       </c>
       <c r="D64" t="n">
-        <v>4.325</v>
+        <v>3.554</v>
       </c>
       <c r="E64" t="n">
-        <v>0.2466</v>
+        <v>0.5497</v>
       </c>
       <c r="F64" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65">
@@ -1718,16 +1718,16 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>0.004142</v>
+        <v>0.009176</v>
       </c>
       <c r="D65" t="n">
-        <v>5.26</v>
+        <v>4.357</v>
       </c>
       <c r="E65" t="n">
-        <v>0.2186</v>
+        <v>0.2289</v>
       </c>
       <c r="F65" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66">
@@ -1738,16 +1738,16 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>0.01208</v>
+        <v>0.002954</v>
       </c>
       <c r="D66" t="n">
-        <v>5.06</v>
+        <v>4.328</v>
       </c>
       <c r="E66" t="n">
-        <v>1.013</v>
+        <v>1.317</v>
       </c>
       <c r="F66" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67">
@@ -1758,16 +1758,16 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>0.01316</v>
+        <v>9.974e-05</v>
       </c>
       <c r="D67" t="n">
-        <v>5.189</v>
+        <v>4.331</v>
       </c>
       <c r="E67" t="n">
-        <v>0.177</v>
+        <v>0.3696</v>
       </c>
       <c r="F67" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68">
@@ -1778,16 +1778,16 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>0.08619</v>
+        <v>0.1508</v>
       </c>
       <c r="D68" t="n">
-        <v>5.176</v>
+        <v>4.494</v>
       </c>
       <c r="E68" t="n">
-        <v>0.1181</v>
+        <v>0.5243</v>
       </c>
       <c r="F68" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69">
@@ -1801,13 +1801,13 @@
         <v>0.006925</v>
       </c>
       <c r="D69" t="n">
-        <v>5.872</v>
+        <v>4.86</v>
       </c>
       <c r="E69" t="n">
         <v>0.1013</v>
       </c>
       <c r="F69" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
@@ -1821,13 +1821,13 @@
         <v>0.02144</v>
       </c>
       <c r="D70" t="n">
-        <v>5.9</v>
+        <v>5.413</v>
       </c>
       <c r="E70" t="n">
         <v>0.0873</v>
       </c>
       <c r="F70" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71">
@@ -1838,16 +1838,16 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>0.01113</v>
+        <v>0.006183</v>
       </c>
       <c r="D71" t="n">
-        <v>6.014</v>
+        <v>5.176</v>
       </c>
       <c r="E71" t="n">
-        <v>0.2145</v>
+        <v>0.5238</v>
       </c>
       <c r="F71" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72">
@@ -1858,16 +1858,16 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>0.02255</v>
+        <v>0.02639</v>
       </c>
       <c r="D72" t="n">
-        <v>6.167</v>
+        <v>5.597</v>
       </c>
       <c r="E72" t="n">
-        <v>0.1816</v>
+        <v>0.3582</v>
       </c>
       <c r="F72" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>